<commit_message>
bullet didn't progress with rounds
</commit_message>
<xml_diff>
--- a/docs/Balance/Balance.xlsx
+++ b/docs/Balance/Balance.xlsx
@@ -15,9 +15,9 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="base_damage">Hoja1!$C$3</definedName>
+    <definedName name="base_damage">Hoja1!$D$3</definedName>
     <definedName name="explosion_shot_base">Hoja1!$F$3</definedName>
-    <definedName name="hits_1_round_behind">Hoja1!$O$1</definedName>
+    <definedName name="hits_1_round_behind">Hoja1!$L$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>tesla trooper life</t>
   </si>
@@ -43,18 +43,6 @@
     <t>explosion shot</t>
   </si>
   <si>
-    <t>damage (cool formula)</t>
-  </si>
-  <si>
-    <t>WEAPONS</t>
-  </si>
-  <si>
-    <t>BASE</t>
-  </si>
-  <si>
-    <t>ENEMIES</t>
-  </si>
-  <si>
     <t>hits to kill 1 round behind</t>
   </si>
   <si>
@@ -62,6 +50,33 @@
   </si>
   <si>
     <t>hits to take down with lvl 1 explosion shot</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Takes</t>
+  </si>
+  <si>
+    <t>hits to kill</t>
+  </si>
+  <si>
+    <t>average weapon damage</t>
+  </si>
+  <si>
+    <t>ENEMY LIFE</t>
+  </si>
+  <si>
+    <t>WEAPON DAMAGE</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$3:$C$12</c:f>
+              <c:f>Hoja1!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -994,13 +1009,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1288,62 +1303,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1351,12 +1375,12 @@
         <f xml:space="preserve"> base_damage</f>
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <f xml:space="preserve"> 100</f>
         <v>100</v>
       </c>
-      <c r="D3">
-        <f>ROUNDUP(B3/base_damage, 0)</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E34" si="0">ROUNDUP(B3/base_damage, 0)</f>
         <v>1</v>
       </c>
       <c r="F3">
@@ -1364,332 +1388,338 @@
         <v>66.666666666666671</v>
       </c>
       <c r="G3">
-        <f>ROUNDUP(B3/explosion_shot_base, 0)</f>
+        <f t="shared" ref="G3:G34" si="1">ROUNDUP(B3/explosion_shot_base, 0)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B61" si="0" xml:space="preserve"> B3 *hits_1_round_behind</f>
+        <f t="shared" ref="B4:B61" si="2" xml:space="preserve"> B3 *hits_1_round_behind</f>
         <v>200</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A3</f>
         <v>200</v>
       </c>
-      <c r="D4">
-        <f>ROUNDUP(B4/base_damage, 0)</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F4">
-        <f>C4/1.75</f>
+        <f>D4/1.75</f>
         <v>114.28571428571429</v>
       </c>
       <c r="G4">
-        <f>ROUNDUP(B4/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A4</f>
         <v>400</v>
       </c>
-      <c r="D5">
-        <f>ROUNDUP(B5/base_damage, 0)</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F61" si="1">C5/1.75</f>
+        <f t="shared" ref="F5:F61" si="3">D5/1.75</f>
         <v>228.57142857142858</v>
       </c>
       <c r="G5">
-        <f>ROUNDUP(B5/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A5</f>
         <v>800</v>
       </c>
-      <c r="D6">
-        <f>ROUNDUP(B6/base_damage, 0)</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>457.14285714285717</v>
       </c>
       <c r="G6">
-        <f>ROUNDUP(B6/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A6</f>
         <v>1600</v>
       </c>
-      <c r="D7">
-        <f>ROUNDUP(B7/base_damage, 0)</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>914.28571428571433</v>
       </c>
       <c r="G7">
-        <f>ROUNDUP(B7/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3200</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A7</f>
         <v>3200</v>
       </c>
-      <c r="D8">
-        <f>ROUNDUP(B8/base_damage, 0)</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1828.5714285714287</v>
       </c>
       <c r="G8">
-        <f>ROUNDUP(B8/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6400</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A8</f>
         <v>6400</v>
       </c>
-      <c r="D9">
-        <f>ROUNDUP(B9/base_damage, 0)</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3657.1428571428573</v>
       </c>
       <c r="G9">
-        <f>ROUNDUP(B9/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12800</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A9</f>
         <v>12800</v>
       </c>
-      <c r="D10">
-        <f>ROUNDUP(B10/base_damage, 0)</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7314.2857142857147</v>
       </c>
       <c r="G10">
-        <f>ROUNDUP(B10/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25600</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A10</f>
         <v>25600</v>
       </c>
-      <c r="D11">
-        <f>ROUNDUP(B11/base_damage, 0)</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14628.571428571429</v>
       </c>
       <c r="G11">
-        <f>ROUNDUP(B11/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>384</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>51200</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A11</f>
         <v>51200</v>
       </c>
-      <c r="D12">
-        <f>ROUNDUP(B12/base_damage, 0)</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29257.142857142859</v>
       </c>
       <c r="G12">
-        <f>ROUNDUP(B12/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>768</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>102400</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A12</f>
         <v>102400</v>
       </c>
-      <c r="D13">
-        <f>ROUNDUP(B13/base_damage, 0)</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>58514.285714285717</v>
       </c>
       <c r="G13">
-        <f>ROUNDUP(B13/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>1536</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>204800</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A13</f>
         <v>204800</v>
       </c>
-      <c r="D14">
-        <f>ROUNDUP(B14/base_damage, 0)</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>2048</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>117028.57142857143</v>
       </c>
       <c r="G14">
-        <f>ROUNDUP(B14/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>3072</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>409600</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A14</f>
         <v>409600</v>
       </c>
-      <c r="D15">
-        <f>ROUNDUP(B15/base_damage, 0)</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>4096</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>234057.14285714287</v>
       </c>
       <c r="G15">
-        <f>ROUNDUP(B15/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>6144</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>819200</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A15</f>
         <v>819200</v>
       </c>
-      <c r="D16">
-        <f>ROUNDUP(B16/base_damage, 0)</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>8192</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>468114.28571428574</v>
       </c>
       <c r="G16">
-        <f>ROUNDUP(B16/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>12288</v>
       </c>
     </row>
@@ -1698,23 +1728,23 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1638400</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A16</f>
         <v>1638400</v>
       </c>
-      <c r="D17">
-        <f>ROUNDUP(B17/base_damage, 0)</f>
+      <c r="E17">
+        <f t="shared" si="0"/>
         <v>16384</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>936228.57142857148</v>
       </c>
       <c r="G17">
-        <f>ROUNDUP(B17/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>24576</v>
       </c>
     </row>
@@ -1723,23 +1753,23 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3276800</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A17</f>
         <v>3276800</v>
       </c>
-      <c r="D18">
-        <f>ROUNDUP(B18/base_damage, 0)</f>
+      <c r="E18">
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1872457.142857143</v>
       </c>
       <c r="G18">
-        <f>ROUNDUP(B18/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>49152</v>
       </c>
     </row>
@@ -1748,23 +1778,23 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6553600</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A18</f>
         <v>6553600</v>
       </c>
-      <c r="D19">
-        <f>ROUNDUP(B19/base_damage, 0)</f>
+      <c r="E19">
+        <f t="shared" si="0"/>
         <v>65536</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3744914.2857142859</v>
       </c>
       <c r="G19">
-        <f>ROUNDUP(B19/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>98304</v>
       </c>
     </row>
@@ -1773,23 +1803,23 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13107200</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A19</f>
         <v>13107200</v>
       </c>
-      <c r="D20">
-        <f>ROUNDUP(B20/base_damage, 0)</f>
+      <c r="E20">
+        <f t="shared" si="0"/>
         <v>131072</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7489828.5714285718</v>
       </c>
       <c r="G20">
-        <f>ROUNDUP(B20/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>196608</v>
       </c>
     </row>
@@ -1798,23 +1828,23 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26214400</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A20</f>
         <v>26214400</v>
       </c>
-      <c r="D21">
-        <f>ROUNDUP(B21/base_damage, 0)</f>
+      <c r="E21">
+        <f t="shared" si="0"/>
         <v>262144</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14979657.142857144</v>
       </c>
       <c r="G21">
-        <f>ROUNDUP(B21/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>393216</v>
       </c>
     </row>
@@ -1823,23 +1853,23 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52428800</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A21</f>
         <v>52428800</v>
       </c>
-      <c r="D22">
-        <f>ROUNDUP(B22/base_damage, 0)</f>
+      <c r="E22">
+        <f t="shared" si="0"/>
         <v>524288</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29959314.285714287</v>
       </c>
       <c r="G22">
-        <f>ROUNDUP(B22/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>786432</v>
       </c>
     </row>
@@ -1848,23 +1878,23 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>104857600</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A22</f>
         <v>104857600</v>
       </c>
-      <c r="D23">
-        <f>ROUNDUP(B23/base_damage, 0)</f>
+      <c r="E23">
+        <f t="shared" si="0"/>
         <v>1048576</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>59918628.571428575</v>
       </c>
       <c r="G23">
-        <f>ROUNDUP(B23/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>1572864</v>
       </c>
     </row>
@@ -1873,23 +1903,23 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>209715200</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A23</f>
         <v>209715200</v>
       </c>
-      <c r="D24">
-        <f>ROUNDUP(B24/base_damage, 0)</f>
+      <c r="E24">
+        <f t="shared" si="0"/>
         <v>2097152</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>119837257.14285715</v>
       </c>
       <c r="G24">
-        <f>ROUNDUP(B24/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>3145728</v>
       </c>
     </row>
@@ -1898,23 +1928,23 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>419430400</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A24</f>
         <v>419430400</v>
       </c>
-      <c r="D25">
-        <f>ROUNDUP(B25/base_damage, 0)</f>
+      <c r="E25">
+        <f t="shared" si="0"/>
         <v>4194304</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>239674514.2857143</v>
       </c>
       <c r="G25">
-        <f>ROUNDUP(B25/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>6291456</v>
       </c>
     </row>
@@ -1923,23 +1953,23 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>838860800</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A25</f>
         <v>838860800</v>
       </c>
-      <c r="D26">
-        <f>ROUNDUP(B26/base_damage, 0)</f>
+      <c r="E26">
+        <f t="shared" si="0"/>
         <v>8388608</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>479349028.5714286</v>
       </c>
       <c r="G26">
-        <f>ROUNDUP(B26/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>12582912</v>
       </c>
     </row>
@@ -1948,23 +1978,23 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1677721600</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A26</f>
         <v>1677721600</v>
       </c>
-      <c r="D27">
-        <f>ROUNDUP(B27/base_damage, 0)</f>
+      <c r="E27">
+        <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>958698057.14285719</v>
       </c>
       <c r="G27">
-        <f>ROUNDUP(B27/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>25165824</v>
       </c>
     </row>
@@ -1973,23 +2003,23 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3355443200</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A27</f>
         <v>3355443200</v>
       </c>
-      <c r="D28">
-        <f>ROUNDUP(B28/base_damage, 0)</f>
+      <c r="E28">
+        <f t="shared" si="0"/>
         <v>33554432</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1917396114.2857144</v>
       </c>
       <c r="G28">
-        <f>ROUNDUP(B28/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>50331648</v>
       </c>
     </row>
@@ -1998,23 +2028,23 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6710886400</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A28</f>
         <v>6710886400</v>
       </c>
-      <c r="D29">
-        <f>ROUNDUP(B29/base_damage, 0)</f>
+      <c r="E29">
+        <f t="shared" si="0"/>
         <v>67108864</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3834792228.5714288</v>
       </c>
       <c r="G29">
-        <f>ROUNDUP(B29/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>100663296</v>
       </c>
     </row>
@@ -2023,23 +2053,23 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13421772800</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A29</f>
         <v>13421772800</v>
       </c>
-      <c r="D30">
-        <f>ROUNDUP(B30/base_damage, 0)</f>
+      <c r="E30">
+        <f t="shared" si="0"/>
         <v>134217728</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7669584457.1428576</v>
       </c>
       <c r="G30">
-        <f>ROUNDUP(B30/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>201326592</v>
       </c>
     </row>
@@ -2048,23 +2078,23 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26843545600</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A30</f>
         <v>26843545600</v>
       </c>
-      <c r="D31">
-        <f>ROUNDUP(B31/base_damage, 0)</f>
+      <c r="E31">
+        <f t="shared" si="0"/>
         <v>268435456</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15339168914.285715</v>
       </c>
       <c r="G31">
-        <f>ROUNDUP(B31/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>402653184</v>
       </c>
     </row>
@@ -2073,23 +2103,23 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>53687091200</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A31</f>
         <v>53687091200</v>
       </c>
-      <c r="D32">
-        <f>ROUNDUP(B32/base_damage, 0)</f>
+      <c r="E32">
+        <f t="shared" si="0"/>
         <v>536870912</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30678337828.57143</v>
       </c>
       <c r="G32">
-        <f>ROUNDUP(B32/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>805306368</v>
       </c>
     </row>
@@ -2098,23 +2128,23 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>107374182400</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A32</f>
         <v>107374182400</v>
       </c>
-      <c r="D33">
-        <f>ROUNDUP(B33/base_damage, 0)</f>
+      <c r="E33">
+        <f t="shared" si="0"/>
         <v>1073741824</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>61356675657.14286</v>
       </c>
       <c r="G33">
-        <f>ROUNDUP(B33/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>1610612736</v>
       </c>
     </row>
@@ -2123,23 +2153,23 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>214748364800</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A33</f>
         <v>214748364800</v>
       </c>
-      <c r="D34">
-        <f>ROUNDUP(B34/base_damage, 0)</f>
+      <c r="E34">
+        <f t="shared" si="0"/>
         <v>2147483648</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>122713351314.28572</v>
       </c>
       <c r="G34">
-        <f>ROUNDUP(B34/explosion_shot_base, 0)</f>
+        <f t="shared" si="1"/>
         <v>3221225472</v>
       </c>
     </row>
@@ -2148,23 +2178,23 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>429496729600</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A34</f>
         <v>429496729600</v>
       </c>
-      <c r="D35">
-        <f>ROUNDUP(B35/base_damage, 0)</f>
+      <c r="E35">
+        <f t="shared" ref="E35:E61" si="4">ROUNDUP(B35/base_damage, 0)</f>
         <v>4294967296</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>245426702628.57144</v>
       </c>
       <c r="G35">
-        <f>ROUNDUP(B35/explosion_shot_base, 0)</f>
+        <f t="shared" ref="G35:G61" si="5">ROUNDUP(B35/explosion_shot_base, 0)</f>
         <v>6442450944</v>
       </c>
     </row>
@@ -2173,23 +2203,23 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>858993459200</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A35</f>
         <v>858993459200</v>
       </c>
-      <c r="D36">
-        <f>ROUNDUP(B36/base_damage, 0)</f>
+      <c r="E36">
+        <f t="shared" si="4"/>
         <v>8589934592</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>490853405257.14288</v>
       </c>
       <c r="G36">
-        <f>ROUNDUP(B36/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>12884901888</v>
       </c>
     </row>
@@ -2198,23 +2228,23 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1717986918400</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A36</f>
         <v>1717986918400</v>
       </c>
-      <c r="D37">
-        <f>ROUNDUP(B37/base_damage, 0)</f>
+      <c r="E37">
+        <f t="shared" si="4"/>
         <v>17179869184</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>981706810514.28577</v>
       </c>
       <c r="G37">
-        <f>ROUNDUP(B37/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>25769803776</v>
       </c>
     </row>
@@ -2223,23 +2253,23 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3435973836800</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A37</f>
         <v>3435973836800</v>
       </c>
-      <c r="D38">
-        <f>ROUNDUP(B38/base_damage, 0)</f>
+      <c r="E38">
+        <f t="shared" si="4"/>
         <v>34359738368</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1963413621028.5715</v>
       </c>
       <c r="G38">
-        <f>ROUNDUP(B38/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>51539607552</v>
       </c>
     </row>
@@ -2248,23 +2278,23 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6871947673600</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A38</f>
         <v>6871947673600</v>
       </c>
-      <c r="D39">
-        <f>ROUNDUP(B39/base_damage, 0)</f>
+      <c r="E39">
+        <f t="shared" si="4"/>
         <v>68719476736</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3926827242057.1431</v>
       </c>
       <c r="G39">
-        <f>ROUNDUP(B39/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>103079215104</v>
       </c>
     </row>
@@ -2273,23 +2303,23 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13743895347200</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A39</f>
         <v>13743895347200</v>
       </c>
-      <c r="D40">
-        <f>ROUNDUP(B40/base_damage, 0)</f>
+      <c r="E40">
+        <f t="shared" si="4"/>
         <v>137438953472</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7853654484114.2861</v>
       </c>
       <c r="G40">
-        <f>ROUNDUP(B40/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>206158430208</v>
       </c>
     </row>
@@ -2298,23 +2328,23 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27487790694400</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A40</f>
         <v>27487790694400</v>
       </c>
-      <c r="D41">
-        <f>ROUNDUP(B41/base_damage, 0)</f>
+      <c r="E41">
+        <f t="shared" si="4"/>
         <v>274877906944</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15707308968228.572</v>
       </c>
       <c r="G41">
-        <f>ROUNDUP(B41/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>412316860416</v>
       </c>
     </row>
@@ -2323,23 +2353,23 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54975581388800</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A41</f>
         <v>54975581388800</v>
       </c>
-      <c r="D42">
-        <f>ROUNDUP(B42/base_damage, 0)</f>
+      <c r="E42">
+        <f t="shared" si="4"/>
         <v>549755813888</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31414617936457.145</v>
       </c>
       <c r="G42">
-        <f>ROUNDUP(B42/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>824633720832</v>
       </c>
     </row>
@@ -2348,23 +2378,23 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>109951162777600</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A42</f>
         <v>109951162777600</v>
       </c>
-      <c r="D43">
-        <f>ROUNDUP(B43/base_damage, 0)</f>
+      <c r="E43">
+        <f t="shared" si="4"/>
         <v>1099511627776</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62829235872914.289</v>
       </c>
       <c r="G43">
-        <f>ROUNDUP(B43/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>1649267441664</v>
       </c>
     </row>
@@ -2373,23 +2403,23 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>219902325555200</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A43</f>
         <v>219902325555200</v>
       </c>
-      <c r="D44">
-        <f>ROUNDUP(B44/base_damage, 0)</f>
+      <c r="E44">
+        <f t="shared" si="4"/>
         <v>2199023255552</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>125658471745828.58</v>
       </c>
       <c r="G44">
-        <f>ROUNDUP(B44/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>3298534883328</v>
       </c>
     </row>
@@ -2398,23 +2428,23 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>439804651110400</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A44</f>
         <v>439804651110400</v>
       </c>
-      <c r="D45">
-        <f>ROUNDUP(B45/base_damage, 0)</f>
+      <c r="E45">
+        <f t="shared" si="4"/>
         <v>4398046511104</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>251316943491657.16</v>
       </c>
       <c r="G45">
-        <f>ROUNDUP(B45/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>6597069766656</v>
       </c>
     </row>
@@ -2423,23 +2453,23 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>879609302220800</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A45</f>
         <v>879609302220800</v>
       </c>
-      <c r="D46">
-        <f>ROUNDUP(B46/base_damage, 0)</f>
+      <c r="E46">
+        <f t="shared" si="4"/>
         <v>8796093022208</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>502633886983314.31</v>
       </c>
       <c r="G46">
-        <f>ROUNDUP(B46/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>13194139533312</v>
       </c>
     </row>
@@ -2448,23 +2478,23 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1759218604441600</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A46</f>
         <v>1759218604441600</v>
       </c>
-      <c r="D47">
-        <f>ROUNDUP(B47/base_damage, 0)</f>
+      <c r="E47">
+        <f t="shared" si="4"/>
         <v>17592186044416</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1005267773966628.6</v>
       </c>
       <c r="G47">
-        <f>ROUNDUP(B47/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>26388279066624</v>
       </c>
     </row>
@@ -2473,23 +2503,23 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3518437208883200</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A47</f>
         <v>3518437208883200</v>
       </c>
-      <c r="D48">
-        <f>ROUNDUP(B48/base_damage, 0)</f>
+      <c r="E48">
+        <f t="shared" si="4"/>
         <v>35184372088832</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2010535547933257.3</v>
       </c>
       <c r="G48">
-        <f>ROUNDUP(B48/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>52776558133248</v>
       </c>
     </row>
@@ -2498,23 +2528,23 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7036874417766400</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A48</f>
         <v>7036874417766400</v>
       </c>
-      <c r="D49">
-        <f>ROUNDUP(B49/base_damage, 0)</f>
+      <c r="E49">
+        <f t="shared" si="4"/>
         <v>70368744177664</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4021071095866514.5</v>
       </c>
       <c r="G49">
-        <f>ROUNDUP(B49/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>105553116266496</v>
       </c>
     </row>
@@ -2523,23 +2553,23 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.40737488355328E+16</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A49</f>
         <v>1.40737488355328E+16</v>
       </c>
-      <c r="D50">
-        <f>ROUNDUP(B50/base_damage, 0)</f>
+      <c r="E50">
+        <f t="shared" si="4"/>
         <v>140737488355328</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8042142191733029</v>
       </c>
       <c r="G50">
-        <f>ROUNDUP(B50/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>211106232532992</v>
       </c>
     </row>
@@ -2548,23 +2578,23 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.81474976710656E+16</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A50</f>
         <v>2.81474976710656E+16</v>
       </c>
-      <c r="D51">
-        <f>ROUNDUP(B51/base_damage, 0)</f>
+      <c r="E51">
+        <f t="shared" si="4"/>
         <v>281474976710656</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6084284383466058E+16</v>
       </c>
       <c r="G51">
-        <f>ROUNDUP(B51/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>422212465065984</v>
       </c>
     </row>
@@ -2573,23 +2603,23 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.62949953421312E+16</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A51</f>
         <v>5.62949953421312E+16</v>
       </c>
-      <c r="D52">
-        <f>ROUNDUP(B52/base_damage, 0)</f>
+      <c r="E52">
+        <f t="shared" si="4"/>
         <v>562949953421312</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2168568766932116E+16</v>
       </c>
       <c r="G52">
-        <f>ROUNDUP(B52/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>844424930131968</v>
       </c>
     </row>
@@ -2598,23 +2628,23 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.125899906842624E+17</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A52</f>
         <v>1.125899906842624E+17</v>
       </c>
-      <c r="D53">
-        <f>ROUNDUP(B53/base_damage, 0)</f>
+      <c r="E53">
+        <f t="shared" si="4"/>
         <v>1125899906842620</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.4337137533864232E+16</v>
       </c>
       <c r="G53">
-        <f>ROUNDUP(B53/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>1688849860263940</v>
       </c>
     </row>
@@ -2623,23 +2653,23 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.251799813685248E+17</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A53</f>
         <v>2.251799813685248E+17</v>
       </c>
-      <c r="D54">
-        <f>ROUNDUP(B54/base_damage, 0)</f>
+      <c r="E54">
+        <f t="shared" si="4"/>
         <v>2251799813685250</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2867427506772846E+17</v>
       </c>
       <c r="G54">
-        <f>ROUNDUP(B54/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>3377699720527870</v>
       </c>
     </row>
@@ -2648,23 +2678,23 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.503599627370496E+17</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A54</f>
         <v>4.503599627370496E+17</v>
       </c>
-      <c r="D55">
-        <f>ROUNDUP(B55/base_damage, 0)</f>
+      <c r="E55">
+        <f t="shared" si="4"/>
         <v>4503599627370500</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5734855013545693E+17</v>
       </c>
       <c r="G55">
-        <f>ROUNDUP(B55/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>6755399441055740</v>
       </c>
     </row>
@@ -2673,23 +2703,23 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.007199254740992E+17</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A55</f>
         <v>9.007199254740992E+17</v>
       </c>
-      <c r="D56">
-        <f>ROUNDUP(B56/base_damage, 0)</f>
+      <c r="E56">
+        <f t="shared" si="4"/>
         <v>9007199254740990</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1469710027091386E+17</v>
       </c>
       <c r="G56">
-        <f>ROUNDUP(B56/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>1.35107988821115E+16</v>
       </c>
     </row>
@@ -2698,23 +2728,23 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.8014398509481984E+18</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A56</f>
         <v>1.8014398509481984E+18</v>
       </c>
-      <c r="D57">
-        <f>ROUNDUP(B57/base_damage, 0)</f>
+      <c r="E57">
+        <f t="shared" si="4"/>
         <v>1.8014398509482E+16</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0293942005418277E+18</v>
       </c>
       <c r="G57">
-        <f>ROUNDUP(B57/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>2.7021597764223E+16</v>
       </c>
     </row>
@@ -2723,23 +2753,23 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6028797018963968E+18</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A57</f>
         <v>3.6028797018963968E+18</v>
       </c>
-      <c r="D58">
-        <f>ROUNDUP(B58/base_damage, 0)</f>
+      <c r="E58">
+        <f t="shared" si="4"/>
         <v>3.6028797018964E+16</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0587884010836554E+18</v>
       </c>
       <c r="G58">
-        <f>ROUNDUP(B58/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>5.4043195528446E+16</v>
       </c>
     </row>
@@ -2748,23 +2778,23 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.2057594037927936E+18</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A58</f>
         <v>7.2057594037927936E+18</v>
       </c>
-      <c r="D59">
-        <f>ROUNDUP(B59/base_damage, 0)</f>
+      <c r="E59">
+        <f t="shared" si="4"/>
         <v>7.2057594037927904E+16</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.1175768021673108E+18</v>
       </c>
       <c r="G59">
-        <f>ROUNDUP(B59/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>1.08086391056892E+17</v>
       </c>
     </row>
@@ -2773,23 +2803,23 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4411518807585587E+19</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A59</f>
         <v>1.4411518807585587E+19</v>
       </c>
-      <c r="D60">
-        <f>ROUNDUP(B60/base_damage, 0)</f>
+      <c r="E60">
+        <f t="shared" si="4"/>
         <v>1.44115188075856E+17</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.2351536043346217E+18</v>
       </c>
       <c r="G60">
-        <f>ROUNDUP(B60/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>2.16172782113784E+17</v>
       </c>
     </row>
@@ -2798,23 +2828,23 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8823037615171174E+19</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A60</f>
         <v>2.8823037615171174E+19</v>
       </c>
-      <c r="D61">
-        <f>ROUNDUP(B61/base_damage, 0)</f>
+      <c r="E61">
+        <f t="shared" si="4"/>
         <v>2.88230376151712E+17</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6470307208669243E+19</v>
       </c>
       <c r="G61">
-        <f>ROUNDUP(B61/explosion_shot_base, 0)</f>
+        <f t="shared" si="5"/>
         <v>4.32345564227568E+17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding structs with the info each enemy needs
</commit_message>
<xml_diff>
--- a/docs/Balance/Balance.xlsx
+++ b/docs/Balance/Balance.xlsx
@@ -18,9 +18,10 @@
     <sheet name="Hoja5" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="base_damage">Hoja1!$D$3</definedName>
-    <definedName name="explosion_shot_base">Hoja1!$F$3</definedName>
-    <definedName name="hits_1_round_behind">Hoja1!$L$1</definedName>
+    <definedName name="base_damage">Hoja1!$E$3</definedName>
+    <definedName name="brute_life_multiplier">Hoja1!$M$2</definedName>
+    <definedName name="explosion_shot_base">Hoja1!$G$3</definedName>
+    <definedName name="hits_1_round_behind">Hoja1!$M$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>round</t>
   </si>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>average weapon</t>
+  </si>
+  <si>
+    <t>brute</t>
   </si>
 </sst>
 </file>
@@ -319,7 +323,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$12</c:f>
+              <c:f>Hoja1!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1086,13 +1090,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1380,76 +1384,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>1.55</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O2" t="str">
-        <f>D2</f>
+      <c r="P2" t="str">
+        <f>E2</f>
         <v>average weapon</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1457,1494 +1471,1730 @@
         <f xml:space="preserve"> base_damage</f>
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="C3">
+        <f xml:space="preserve"> $B$3*brute_life_multiplier</f>
+        <v>1500</v>
+      </c>
+      <c r="E3">
         <f xml:space="preserve"> 100</f>
         <v>100</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E34" si="0">ROUNDUP(B3/base_damage, 0)</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F34" si="0">ROUNDUP(B3/base_damage, 0)</f>
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <f>base_damage/2</f>
         <v>50</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G34" si="1">ROUNDUP(B3/explosion_shot_base, 0)</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H34" si="1">ROUNDUP(B3/explosion_shot_base, 0)</f>
         <v>2</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <f>B2</f>
         <v>tesla trooper</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B61" si="2" xml:space="preserve"> B3 *hits_1_round_behind</f>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A3</f>
         <v>155</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D35" si="3" xml:space="preserve"> base_damage * hits_1_round_behind ^ A3</f>
+      <c r="C4">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A3*brute_life_multiplier</f>
+        <v>2325</v>
+      </c>
+      <c r="E4">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A3</f>
         <v>155</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F4">
-        <f>D4/2</f>
+      <c r="G4">
+        <f>E4/2</f>
         <v>77.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O4" t="str">
-        <f ca="1">OFFSET(O2,1, 0)</f>
+      <c r="P4" t="str">
+        <f ca="1">OFFSET(P2,1, 0)</f>
         <v>tesla trooper</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
-        <v>240.25</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A4</f>
         <v>240.25000000000003</v>
       </c>
+      <c r="C5">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A4*brute_life_multiplier</f>
+        <v>3603.7500000000005</v>
+      </c>
       <c r="E5">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A4</f>
+        <v>240.25000000000003</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F61" si="4">D5/2</f>
+      <c r="G5">
+        <f t="shared" ref="G5:G61" si="2">E5/2</f>
         <v>120.12500000000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
-        <v>372.38749999999999</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A5</f>
         <v>372.38750000000005</v>
       </c>
+      <c r="C6">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A5*brute_life_multiplier</f>
+        <v>5585.8125000000009</v>
+      </c>
       <c r="E6">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A5</f>
+        <v>372.38750000000005</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="4"/>
+      <c r="G6">
+        <f t="shared" si="2"/>
         <v>186.19375000000002</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
-        <v>577.20062499999995</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A6</f>
         <v>577.20062500000017</v>
       </c>
+      <c r="C7">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A6*brute_life_multiplier</f>
+        <v>8658.0093750000033</v>
+      </c>
       <c r="E7">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A6</f>
+        <v>577.20062500000017</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="4"/>
+      <c r="G7">
+        <f t="shared" si="2"/>
         <v>288.60031250000009</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" si="2"/>
-        <v>894.66096874999994</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A7</f>
         <v>894.66096875000028</v>
       </c>
+      <c r="C8">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A7*brute_life_multiplier</f>
+        <v>13419.914531250004</v>
+      </c>
       <c r="E8">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A7</f>
+        <v>894.66096875000028</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
+      <c r="G8">
+        <f t="shared" si="2"/>
         <v>447.33048437500014</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="2"/>
-        <v>1386.7245015624999</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A8</f>
         <v>1386.7245015625006</v>
       </c>
+      <c r="C9">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A8*brute_life_multiplier</f>
+        <v>20800.867523437508</v>
+      </c>
       <c r="E9">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A8</f>
+        <v>1386.7245015625006</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
+      <c r="G9">
+        <f t="shared" si="2"/>
         <v>693.36225078125028</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
-        <v>2149.4229774218747</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A9</f>
         <v>2149.4229774218761</v>
       </c>
+      <c r="C10">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A9*brute_life_multiplier</f>
+        <v>32241.344661328141</v>
+      </c>
       <c r="E10">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A9</f>
+        <v>2149.4229774218761</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
+      <c r="G10">
+        <f t="shared" si="2"/>
         <v>1074.7114887109381</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
-        <v>3331.6056150039058</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A10</f>
         <v>3331.605615003908</v>
       </c>
+      <c r="C11">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A10*brute_life_multiplier</f>
+        <v>49974.084225058621</v>
+      </c>
       <c r="E11">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A10</f>
+        <v>3331.605615003908</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
+      <c r="G11">
+        <f t="shared" si="2"/>
         <v>1665.802807501954</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
-        <v>5163.9887032560537</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A11</f>
         <v>5163.9887032560582</v>
       </c>
+      <c r="C12">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A11*brute_life_multiplier</f>
+        <v>77459.830548840866</v>
+      </c>
       <c r="E12">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A11</f>
+        <v>5163.9887032560582</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
+      <c r="G12">
+        <f t="shared" si="2"/>
         <v>2581.9943516280291</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" si="2"/>
-        <v>8004.1824900468837</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A12</f>
         <v>8004.1824900468891</v>
       </c>
+      <c r="C13">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A12*brute_life_multiplier</f>
+        <v>120062.73735070333</v>
+      </c>
       <c r="E13">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A12</f>
+        <v>8004.1824900468891</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
+      <c r="G13">
+        <f t="shared" si="2"/>
         <v>4002.0912450234446</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="2"/>
-        <v>12406.48285957267</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A13</f>
         <v>12406.482859572679</v>
       </c>
+      <c r="C14">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A13*brute_life_multiplier</f>
+        <v>186097.24289359018</v>
+      </c>
       <c r="E14">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A13</f>
+        <v>12406.482859572679</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
+      <c r="G14">
+        <f t="shared" si="2"/>
         <v>6203.2414297863397</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" si="2"/>
-        <v>19230.04843233764</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A14</f>
         <v>19230.048432337655</v>
       </c>
+      <c r="C15">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A14*brute_life_multiplier</f>
+        <v>288450.72648506484</v>
+      </c>
       <c r="E15">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A14</f>
+        <v>19230.048432337655</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>193</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
+      <c r="G15">
+        <f t="shared" si="2"/>
         <v>9615.0242161688275</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="2"/>
-        <v>29806.575070123345</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A15</f>
         <v>29806.57507012337</v>
       </c>
+      <c r="C16">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A15*brute_life_multiplier</f>
+        <v>447098.62605185056</v>
+      </c>
       <c r="E16">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A15</f>
+        <v>29806.57507012337</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>299</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
+      <c r="G16">
+        <f t="shared" si="2"/>
         <v>14903.287535061685</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>597</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="2"/>
-        <v>46200.191358691183</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A16</f>
         <v>46200.191358691227</v>
       </c>
+      <c r="C17">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A16*brute_life_multiplier</f>
+        <v>693002.87038036843</v>
+      </c>
       <c r="E17">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A16</f>
+        <v>46200.191358691227</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="0"/>
         <v>463</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
+      <c r="G17">
+        <f t="shared" si="2"/>
         <v>23100.095679345613</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>925</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" si="2"/>
-        <v>71610.296605971336</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A17</f>
         <v>71610.296605971409</v>
       </c>
+      <c r="C18">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A17*brute_life_multiplier</f>
+        <v>1074154.4490895711</v>
+      </c>
       <c r="E18">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A17</f>
+        <v>71610.296605971409</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>717</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
+      <c r="G18">
+        <f t="shared" si="2"/>
         <v>35805.148302985705</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>1433</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
-        <v>110995.95973925557</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A18</f>
         <v>110995.95973925568</v>
       </c>
+      <c r="C19">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A18*brute_life_multiplier</f>
+        <v>1664939.3960888351</v>
+      </c>
       <c r="E19">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A18</f>
+        <v>110995.95973925568</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="0"/>
         <v>1110</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
+      <c r="G19">
+        <f t="shared" si="2"/>
         <v>55497.979869627838</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>2220</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
-        <v>172043.73759584615</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A19</f>
         <v>172043.73759584629</v>
       </c>
+      <c r="C20">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A19*brute_life_multiplier</f>
+        <v>2580656.0639376943</v>
+      </c>
       <c r="E20">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A19</f>
+        <v>172043.73759584629</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>1721</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
+      <c r="G20">
+        <f t="shared" si="2"/>
         <v>86021.868797923147</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="1"/>
         <v>3441</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="2"/>
-        <v>266667.79327356152</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A20</f>
         <v>266667.79327356181</v>
       </c>
+      <c r="C21">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A20*brute_life_multiplier</f>
+        <v>4000016.8991034273</v>
+      </c>
       <c r="E21">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A20</f>
+        <v>266667.79327356181</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>2667</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
+      <c r="G21">
+        <f t="shared" si="2"/>
         <v>133333.8966367809</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="1"/>
         <v>5334</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
-        <v>413335.07957402035</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A21</f>
         <v>413335.07957402081</v>
       </c>
+      <c r="C22">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A21*brute_life_multiplier</f>
+        <v>6200026.1936103124</v>
+      </c>
       <c r="E22">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A21</f>
+        <v>413335.07957402081</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
         <v>4134</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
+      <c r="G22">
+        <f t="shared" si="2"/>
         <v>206667.53978701041</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="1"/>
         <v>8267</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <f t="shared" si="2"/>
-        <v>640669.3733397316</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A22</f>
         <v>640669.37333973229</v>
       </c>
+      <c r="C23">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A22*brute_life_multiplier</f>
+        <v>9610040.6000959836</v>
+      </c>
       <c r="E23">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A22</f>
+        <v>640669.37333973229</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="0"/>
         <v>6407</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
+      <c r="G23">
+        <f t="shared" si="2"/>
         <v>320334.68666986615</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="1"/>
         <v>12814</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <f t="shared" si="2"/>
-        <v>993037.52867658401</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A23</f>
         <v>993037.52867658518</v>
       </c>
+      <c r="C24">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A23*brute_life_multiplier</f>
+        <v>14895562.930148778</v>
+      </c>
       <c r="E24">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A23</f>
+        <v>993037.52867658518</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="0"/>
         <v>9931</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
+      <c r="G24">
+        <f t="shared" si="2"/>
         <v>496518.76433829259</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="1"/>
         <v>19861</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <f t="shared" si="2"/>
-        <v>1539208.1694487052</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A24</f>
         <v>1539208.169448707</v>
       </c>
+      <c r="C25">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A24*brute_life_multiplier</f>
+        <v>23088122.541730605</v>
+      </c>
       <c r="E25">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A24</f>
+        <v>1539208.169448707</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="0"/>
         <v>15393</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
+      <c r="G25">
+        <f t="shared" si="2"/>
         <v>769604.08472435351</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="1"/>
         <v>30785</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <f t="shared" si="2"/>
-        <v>2385772.6626454932</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A25</f>
         <v>2385772.662645496</v>
       </c>
+      <c r="C26">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A25*brute_life_multiplier</f>
+        <v>35786589.939682439</v>
+      </c>
       <c r="E26">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A25</f>
+        <v>2385772.662645496</v>
+      </c>
+      <c r="F26">
         <f t="shared" si="0"/>
         <v>23858</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
+      <c r="G26">
+        <f t="shared" si="2"/>
         <v>1192886.331322748</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="1"/>
         <v>47716</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <f t="shared" si="2"/>
-        <v>3697947.6271005147</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A26</f>
         <v>3697947.6271005194</v>
       </c>
+      <c r="C27">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A26*brute_life_multiplier</f>
+        <v>55469214.40650779</v>
+      </c>
       <c r="E27">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A26</f>
+        <v>3697947.6271005194</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="0"/>
         <v>36980</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
+      <c r="G27">
+        <f t="shared" si="2"/>
         <v>1848973.8135502597</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="1"/>
         <v>73959</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <f t="shared" si="2"/>
-        <v>5731818.8220057981</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A27</f>
         <v>5731818.8220058056</v>
       </c>
+      <c r="C28">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A27*brute_life_multiplier</f>
+        <v>85977282.330087081</v>
+      </c>
       <c r="E28">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A27</f>
+        <v>5731818.8220058056</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="0"/>
         <v>57319</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
+      <c r="G28">
+        <f t="shared" si="2"/>
         <v>2865909.4110029028</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="1"/>
         <v>114637</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <f t="shared" si="2"/>
-        <v>8884319.1741089877</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A28</f>
         <v>8884319.1741089988</v>
       </c>
+      <c r="C29">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A28*brute_life_multiplier</f>
+        <v>133264787.61163498</v>
+      </c>
       <c r="E29">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A28</f>
+        <v>8884319.1741089988</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="0"/>
         <v>88844</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
+      <c r="G29">
+        <f t="shared" si="2"/>
         <v>4442159.5870544994</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="1"/>
         <v>177687</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <f t="shared" si="2"/>
-        <v>13770694.719868932</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A29</f>
         <v>13770694.719868949</v>
       </c>
+      <c r="C30">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A29*brute_life_multiplier</f>
+        <v>206560420.79803422</v>
+      </c>
       <c r="E30">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A29</f>
+        <v>13770694.719868949</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>137707</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="4"/>
+      <c r="G30">
+        <f t="shared" si="2"/>
         <v>6885347.3599344743</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="1"/>
         <v>275414</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
-        <v>21344576.815796845</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A30</f>
         <v>21344576.815796874</v>
       </c>
+      <c r="C31">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A30*brute_life_multiplier</f>
+        <v>320168652.23695314</v>
+      </c>
       <c r="E31">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A30</f>
+        <v>21344576.815796874</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="0"/>
         <v>213446</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="4"/>
+      <c r="G31">
+        <f t="shared" si="2"/>
         <v>10672288.407898437</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="1"/>
         <v>426892</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
-        <v>33084094.06448511</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A31</f>
         <v>33084094.064485155</v>
       </c>
+      <c r="C32">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A31*brute_life_multiplier</f>
+        <v>496261410.96727735</v>
+      </c>
       <c r="E32">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A31</f>
+        <v>33084094.064485155</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="0"/>
         <v>330841</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
+      <c r="G32">
+        <f t="shared" si="2"/>
         <v>16542047.032242578</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="1"/>
         <v>661682</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
-        <v>51280345.799951926</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A32</f>
         <v>51280345.799952</v>
       </c>
+      <c r="C33">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A32*brute_life_multiplier</f>
+        <v>769205186.99927998</v>
+      </c>
       <c r="E33">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A32</f>
+        <v>51280345.799952</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="0"/>
         <v>512804</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="4"/>
+      <c r="G33">
+        <f t="shared" si="2"/>
         <v>25640172.899976</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="1"/>
         <v>1025607</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
-        <v>79484535.989925489</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A33</f>
         <v>79484535.989925608</v>
       </c>
+      <c r="C34">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A33*brute_life_multiplier</f>
+        <v>1192268039.8488841</v>
+      </c>
       <c r="E34">
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A33</f>
+        <v>79484535.989925608</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="0"/>
         <v>794846</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="4"/>
+      <c r="G34">
+        <f t="shared" si="2"/>
         <v>39742267.994962804</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="1"/>
         <v>1589691</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
-        <v>123201030.7843845</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A34</f>
         <v>123201030.78438467</v>
       </c>
+      <c r="C35">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A34*brute_life_multiplier</f>
+        <v>1848015461.76577</v>
+      </c>
       <c r="E35">
-        <f t="shared" ref="E35:E61" si="5">ROUNDUP(B35/base_damage, 0)</f>
+        <f xml:space="preserve"> base_damage * hits_1_round_behind ^ A34</f>
+        <v>123201030.78438467</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F61" si="3">ROUNDUP(B35/base_damage, 0)</f>
         <v>1232011</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="4"/>
+      <c r="G35">
+        <f t="shared" si="2"/>
         <v>61600515.392192334</v>
       </c>
-      <c r="G35">
-        <f t="shared" ref="G35:G61" si="6">ROUNDUP(B35/explosion_shot_base, 0)</f>
+      <c r="H35">
+        <f t="shared" ref="H35:H61" si="4">ROUNDUP(B35/explosion_shot_base, 0)</f>
         <v>2464021</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
-        <v>190961597.71579599</v>
-      </c>
-      <c r="D36">
-        <f t="shared" ref="D36:D61" si="7" xml:space="preserve"> base_damage * hits_1_round_behind ^ A35</f>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A35</f>
         <v>190961597.71579626</v>
       </c>
+      <c r="C36">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A35*brute_life_multiplier</f>
+        <v>2864423965.7369437</v>
+      </c>
       <c r="E36">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E36:E61" si="5" xml:space="preserve"> base_damage * hits_1_round_behind ^ A35</f>
+        <v>190961597.71579626</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
         <v>1909616</v>
       </c>
-      <c r="F36">
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>95480798.857898131</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="4"/>
-        <v>95480798.857898131</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="6"/>
         <v>3819232</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <f t="shared" si="2"/>
-        <v>295990476.4594838</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A36</f>
         <v>295990476.45948422</v>
+      </c>
+      <c r="C37">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A36*brute_life_multiplier</f>
+        <v>4439857146.8922634</v>
       </c>
       <c r="E37">
         <f t="shared" si="5"/>
+        <v>295990476.45948422</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
         <v>2959905</v>
       </c>
-      <c r="F37">
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>147995238.22974211</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="4"/>
-        <v>147995238.22974211</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="6"/>
         <v>5919810</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <f t="shared" si="2"/>
-        <v>458785238.51219988</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A37</f>
         <v>458785238.51220059</v>
+      </c>
+      <c r="C38">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A37*brute_life_multiplier</f>
+        <v>6881778577.6830091</v>
       </c>
       <c r="E38">
         <f t="shared" si="5"/>
+        <v>458785238.51220059</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
         <v>4587853</v>
       </c>
-      <c r="F38">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>229392619.2561003</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="4"/>
-        <v>229392619.2561003</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="6"/>
         <v>9175705</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <f t="shared" si="2"/>
-        <v>711117119.69390988</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A38</f>
         <v>711117119.69391084</v>
+      </c>
+      <c r="C39">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A38*brute_life_multiplier</f>
+        <v>10666756795.408663</v>
       </c>
       <c r="E39">
         <f t="shared" si="5"/>
+        <v>711117119.69391084</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
         <v>7111172</v>
       </c>
-      <c r="F39">
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>355558559.84695542</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="4"/>
-        <v>355558559.84695542</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="6"/>
         <v>14222343</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
-        <v>1102231535.5255604</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A39</f>
         <v>1102231535.5255618</v>
+      </c>
+      <c r="C40">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A39*brute_life_multiplier</f>
+        <v>16533473032.883427</v>
       </c>
       <c r="E40">
         <f t="shared" si="5"/>
+        <v>1102231535.5255618</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
         <v>11022316</v>
       </c>
-      <c r="F40">
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>551115767.7627809</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="4"/>
-        <v>551115767.7627809</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="6"/>
         <v>22044631</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <f t="shared" si="2"/>
-        <v>1708458880.0646186</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A40</f>
         <v>1708458880.0646212</v>
+      </c>
+      <c r="C41">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A40*brute_life_multiplier</f>
+        <v>25626883200.969318</v>
       </c>
       <c r="E41">
         <f t="shared" si="5"/>
+        <v>1708458880.0646212</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="3"/>
         <v>17084589</v>
       </c>
-      <c r="F41">
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>854229440.03231061</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="4"/>
-        <v>854229440.03231061</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="6"/>
         <v>34169178</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <f t="shared" si="2"/>
-        <v>2648111264.1001587</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A41</f>
         <v>2648111264.100163</v>
+      </c>
+      <c r="C42">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A41*brute_life_multiplier</f>
+        <v>39721668961.502441</v>
       </c>
       <c r="E42">
         <f t="shared" si="5"/>
+        <v>2648111264.100163</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="3"/>
         <v>26481113</v>
       </c>
-      <c r="F42">
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>1324055632.0500815</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="4"/>
-        <v>1324055632.0500815</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="6"/>
         <v>52962226</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <f t="shared" si="2"/>
-        <v>4104572459.3552461</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A42</f>
         <v>4104572459.3552532</v>
+      </c>
+      <c r="C43">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A42*brute_life_multiplier</f>
+        <v>61568586890.328796</v>
       </c>
       <c r="E43">
         <f t="shared" si="5"/>
+        <v>4104572459.3552532</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="3"/>
         <v>41045725</v>
       </c>
-      <c r="F43">
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>2052286229.6776266</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="4"/>
-        <v>2052286229.6776266</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="6"/>
         <v>82091450</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <f t="shared" si="2"/>
-        <v>6362087312.0006313</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A43</f>
         <v>6362087312.0006428</v>
+      </c>
+      <c r="C44">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A43*brute_life_multiplier</f>
+        <v>95431309680.009644</v>
       </c>
       <c r="E44">
         <f t="shared" si="5"/>
+        <v>6362087312.0006428</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="3"/>
         <v>63620874</v>
       </c>
-      <c r="F44">
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>3181043656.0003214</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="4"/>
-        <v>3181043656.0003214</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="6"/>
         <v>127241747</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <f t="shared" si="2"/>
-        <v>9861235333.6009789</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A44</f>
         <v>9861235333.600996</v>
+      </c>
+      <c r="C45">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A44*brute_life_multiplier</f>
+        <v>147918530004.01495</v>
       </c>
       <c r="E45">
         <f t="shared" si="5"/>
+        <v>9861235333.600996</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
         <v>98612354</v>
       </c>
-      <c r="F45">
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>4930617666.800498</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="4"/>
-        <v>4930617666.800498</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="6"/>
         <v>197224707</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
-        <f t="shared" si="2"/>
-        <v>15284914767.081518</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A45</f>
         <v>15284914767.081543</v>
+      </c>
+      <c r="C46">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A45*brute_life_multiplier</f>
+        <v>229273721506.22314</v>
       </c>
       <c r="E46">
         <f t="shared" si="5"/>
+        <v>15284914767.081543</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="3"/>
         <v>152849148</v>
       </c>
-      <c r="F46">
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>7642457383.5407715</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="4"/>
-        <v>7642457383.5407715</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="6"/>
         <v>305698296</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <f t="shared" si="2"/>
-        <v>23691617888.976353</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A46</f>
         <v>23691617888.976398</v>
+      </c>
+      <c r="C47">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A46*brute_life_multiplier</f>
+        <v>355374268334.646</v>
       </c>
       <c r="E47">
         <f t="shared" si="5"/>
+        <v>23691617888.976398</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="3"/>
         <v>236916179</v>
       </c>
-      <c r="F47">
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>11845808944.488199</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="4"/>
-        <v>11845808944.488199</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="6"/>
         <v>473832358</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <f t="shared" si="2"/>
-        <v>36722007727.913345</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A47</f>
         <v>36722007727.913422</v>
+      </c>
+      <c r="C48">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A47*brute_life_multiplier</f>
+        <v>550830115918.70129</v>
       </c>
       <c r="E48">
         <f t="shared" si="5"/>
+        <v>36722007727.913422</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
         <v>367220078</v>
       </c>
-      <c r="F48">
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>18361003863.956711</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="4"/>
-        <v>18361003863.956711</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="6"/>
         <v>734440155</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <f t="shared" si="2"/>
-        <v>56919111978.265686</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A48</f>
         <v>56919111978.265808</v>
+      </c>
+      <c r="C49">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A48*brute_life_multiplier</f>
+        <v>853786679673.98706</v>
       </c>
       <c r="E49">
         <f t="shared" si="5"/>
+        <v>56919111978.265808</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
         <v>569191120</v>
       </c>
-      <c r="F49">
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>28459555989.132904</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="4"/>
-        <v>28459555989.132904</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="6"/>
         <v>1138382240</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <f t="shared" si="2"/>
-        <v>88224623566.311813</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A49</f>
         <v>88224623566.311996</v>
+      </c>
+      <c r="C50">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A49*brute_life_multiplier</f>
+        <v>1323369353494.6799</v>
       </c>
       <c r="E50">
         <f t="shared" si="5"/>
+        <v>88224623566.311996</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
         <v>882246236</v>
       </c>
-      <c r="F50">
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>44112311783.155998</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="4"/>
-        <v>44112311783.155998</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="6"/>
         <v>1764492472</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <f t="shared" si="2"/>
-        <v>136748166527.78331</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A50</f>
         <v>136748166527.78362</v>
+      </c>
+      <c r="C51">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A50*brute_life_multiplier</f>
+        <v>2051222497916.7542</v>
       </c>
       <c r="E51">
         <f t="shared" si="5"/>
+        <v>136748166527.78362</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
         <v>1367481666</v>
       </c>
-      <c r="F51">
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>68374083263.891808</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="4"/>
-        <v>68374083263.891808</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="6"/>
         <v>2734963331</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <f t="shared" si="2"/>
-        <v>211959658118.06415</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A51</f>
         <v>211959658118.06461</v>
+      </c>
+      <c r="C52">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A51*brute_life_multiplier</f>
+        <v>3179394871770.9692</v>
       </c>
       <c r="E52">
         <f t="shared" si="5"/>
+        <v>211959658118.06461</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
         <v>2119596582</v>
       </c>
-      <c r="F52">
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>105979829059.0323</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="4"/>
-        <v>105979829059.0323</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="6"/>
         <v>4239193163</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
-        <f t="shared" si="2"/>
-        <v>328537470082.99945</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A52</f>
         <v>328537470083.00012</v>
+      </c>
+      <c r="C53">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A52*brute_life_multiplier</f>
+        <v>4928062051245.002</v>
       </c>
       <c r="E53">
         <f t="shared" si="5"/>
+        <v>328537470083.00012</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
         <v>3285374701</v>
       </c>
-      <c r="F53">
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>164268735041.50006</v>
+      </c>
+      <c r="H53">
         <f t="shared" si="4"/>
-        <v>164268735041.50006</v>
-      </c>
-      <c r="G53">
-        <f t="shared" si="6"/>
         <v>6570749402</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
-        <f t="shared" si="2"/>
-        <v>509233078628.64917</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A53</f>
         <v>509233078628.65027</v>
+      </c>
+      <c r="C54">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A53*brute_life_multiplier</f>
+        <v>7638496179429.7539</v>
       </c>
       <c r="E54">
         <f t="shared" si="5"/>
+        <v>509233078628.65027</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="3"/>
         <v>5092330787</v>
       </c>
-      <c r="F54">
+      <c r="G54">
+        <f t="shared" si="2"/>
+        <v>254616539314.32513</v>
+      </c>
+      <c r="H54">
         <f t="shared" si="4"/>
-        <v>254616539314.32513</v>
-      </c>
-      <c r="G54">
-        <f t="shared" si="6"/>
         <v>10184661573</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
-        <f t="shared" si="2"/>
-        <v>789311271874.40625</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A54</f>
         <v>789311271874.40796</v>
+      </c>
+      <c r="C55">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A54*brute_life_multiplier</f>
+        <v>11839669078116.119</v>
       </c>
       <c r="E55">
         <f t="shared" si="5"/>
+        <v>789311271874.40796</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="3"/>
         <v>7893112719</v>
       </c>
-      <c r="F55">
+      <c r="G55">
+        <f t="shared" si="2"/>
+        <v>394655635937.20398</v>
+      </c>
+      <c r="H55">
         <f t="shared" si="4"/>
-        <v>394655635937.20398</v>
-      </c>
-      <c r="G55">
-        <f t="shared" si="6"/>
         <v>15786225438</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
-        <f t="shared" si="2"/>
-        <v>1223432471405.3298</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A55</f>
         <v>1223432471405.3323</v>
+      </c>
+      <c r="C56">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A55*brute_life_multiplier</f>
+        <v>18351487071079.984</v>
       </c>
       <c r="E56">
         <f t="shared" si="5"/>
+        <v>1223432471405.3323</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="3"/>
         <v>12234324715</v>
       </c>
-      <c r="F56">
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>611716235702.66614</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="4"/>
-        <v>611716235702.66614</v>
-      </c>
-      <c r="G56">
-        <f t="shared" si="6"/>
         <v>24468649429</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
-        <f t="shared" si="2"/>
-        <v>1896320330678.2612</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A56</f>
         <v>1896320330678.2654</v>
+      </c>
+      <c r="C57">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A56*brute_life_multiplier</f>
+        <v>28444804960173.98</v>
       </c>
       <c r="E57">
         <f t="shared" si="5"/>
+        <v>1896320330678.2654</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="3"/>
         <v>18963203307</v>
       </c>
-      <c r="F57">
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>948160165339.13269</v>
+      </c>
+      <c r="H57">
         <f t="shared" si="4"/>
-        <v>948160165339.13269</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="6"/>
         <v>37926406614</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
-        <f t="shared" si="2"/>
-        <v>2939296512551.3052</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A57</f>
         <v>2939296512551.3115</v>
+      </c>
+      <c r="C58">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A57*brute_life_multiplier</f>
+        <v>44089447688269.672</v>
       </c>
       <c r="E58">
         <f t="shared" si="5"/>
+        <v>2939296512551.3115</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="3"/>
         <v>29392965126</v>
       </c>
-      <c r="F58">
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>1469648256275.6558</v>
+      </c>
+      <c r="H58">
         <f t="shared" si="4"/>
-        <v>1469648256275.6558</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="6"/>
         <v>58785930252</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
-        <f t="shared" si="2"/>
-        <v>4555909594454.5234</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A58</f>
         <v>4555909594454.5332</v>
+      </c>
+      <c r="C59">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A58*brute_life_multiplier</f>
+        <v>68338643916818</v>
       </c>
       <c r="E59">
         <f t="shared" si="5"/>
+        <v>4555909594454.5332</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="3"/>
         <v>45559095945</v>
       </c>
-      <c r="F59">
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>2277954797227.2666</v>
+      </c>
+      <c r="H59">
         <f t="shared" si="4"/>
-        <v>2277954797227.2666</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="6"/>
         <v>91118191890</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60">
-        <f t="shared" si="2"/>
-        <v>7061659871404.5117</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A59</f>
         <v>7061659871404.5273</v>
+      </c>
+      <c r="C60">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A59*brute_life_multiplier</f>
+        <v>105924898071067.91</v>
       </c>
       <c r="E60">
         <f t="shared" si="5"/>
+        <v>7061659871404.5273</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="3"/>
         <v>70616598715</v>
       </c>
-      <c r="F60">
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>3530829935702.2637</v>
+      </c>
+      <c r="H60">
         <f t="shared" si="4"/>
-        <v>3530829935702.2637</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="6"/>
         <v>141233197429</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61">
-        <f t="shared" si="2"/>
-        <v>10945572800676.994</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A60</f>
         <v>10945572800677.02</v>
+      </c>
+      <c r="C61">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A60*brute_life_multiplier</f>
+        <v>164183592010155.28</v>
       </c>
       <c r="E61">
         <f t="shared" si="5"/>
+        <v>10945572800677.02</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="3"/>
         <v>109455728007</v>
       </c>
-      <c r="F61">
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>5472786400338.5098</v>
+      </c>
+      <c r="H61">
         <f t="shared" si="4"/>
-        <v>5472786400338.5098</v>
-      </c>
-      <c r="G61">
-        <f t="shared" si="6"/>
         <v>218911456014</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tesla trooper getting values from the balance xml
</commit_message>
<xml_diff>
--- a/docs/Balance/Balance.xlsx
+++ b/docs/Balance/Balance.xlsx
@@ -202,11 +202,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1387,7 +1384,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,37 +1395,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M1">
         <v>1.55</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E2" t="s">
@@ -1437,26 +1437,26 @@
       <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M2">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P2" t="str">
         <f>E2</f>
         <v>average weapon</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="R2">
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f xml:space="preserve"> base_damage</f>
+        <f xml:space="preserve"> base_damage* hits_1_round_behind ^ A2</f>
         <v>100</v>
       </c>
       <c r="C3">
@@ -1491,14 +1491,14 @@
         <f t="shared" ref="H3:H34" si="1">ROUNDUP(B3/explosion_shot_base, 0)</f>
         <v>2</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P3" t="str">
         <f>B2</f>
         <v>tesla trooper</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="R3">
@@ -1533,14 +1533,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="P4" t="str">
         <f ca="1">OFFSET(P2,1, 0)</f>
         <v>tesla trooper</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -4448,7 +4448,7 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>D2</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
loading weapon balance variables from xml
</commit_message>
<xml_diff>
--- a/docs/Balance/Balance.xlsx
+++ b/docs/Balance/Balance.xlsx
@@ -1381,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1395,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3196,6 +3196,1195 @@
       <c r="H61">
         <f t="shared" si="4"/>
         <v>218911456014</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A61</f>
+        <v>16965637841049.377</v>
+      </c>
+      <c r="C62">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A61*brute_life_multiplier</f>
+        <v>254484567615740.66</v>
+      </c>
+      <c r="E62">
+        <f t="shared" ref="E62:E84" si="6" xml:space="preserve"> base_damage * hits_1_round_behind ^ A61</f>
+        <v>16965637841049.377</v>
+      </c>
+      <c r="F62">
+        <f t="shared" ref="F62:F84" si="7">ROUNDUP(B62/base_damage, 0)</f>
+        <v>169656378411</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ref="G62:G84" si="8">E62/2</f>
+        <v>8482818920524.6885</v>
+      </c>
+      <c r="H62">
+        <f t="shared" ref="H62:H84" si="9">ROUNDUP(B62/explosion_shot_base, 0)</f>
+        <v>339312756821</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A62</f>
+        <v>26296738653626.543</v>
+      </c>
+      <c r="C63">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A62*brute_life_multiplier</f>
+        <v>394451079804398.13</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="6"/>
+        <v>26296738653626.543</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="7"/>
+        <v>262967386537</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="8"/>
+        <v>13148369326813.271</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="9"/>
+        <v>525934773073</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A63</f>
+        <v>40759944913121.133</v>
+      </c>
+      <c r="C64">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A63*brute_life_multiplier</f>
+        <v>611399173696817</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="6"/>
+        <v>40759944913121.133</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="7"/>
+        <v>407599449132</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="8"/>
+        <v>20379972456560.566</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="9"/>
+        <v>815198898263</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A64</f>
+        <v>63177914615337.781</v>
+      </c>
+      <c r="C65">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A64*brute_life_multiplier</f>
+        <v>947668719230066.75</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="6"/>
+        <v>63177914615337.781</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="7"/>
+        <v>631779146154</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="8"/>
+        <v>31588957307668.891</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="9"/>
+        <v>1263558292307</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A65</f>
+        <v>97925767653773.563</v>
+      </c>
+      <c r="C66">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A65*brute_life_multiplier</f>
+        <v>1468886514806603.5</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="6"/>
+        <v>97925767653773.563</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="7"/>
+        <v>979257676538</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="8"/>
+        <v>48962883826886.781</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="9"/>
+        <v>1958515353076</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A66</f>
+        <v>151784939863349</v>
+      </c>
+      <c r="C67">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A66*brute_life_multiplier</f>
+        <v>2276774097950235</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="6"/>
+        <v>151784939863349</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="7"/>
+        <v>1517849398634</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="8"/>
+        <v>75892469931674.5</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="9"/>
+        <v>3035698797267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A67</f>
+        <v>235266656788190.97</v>
+      </c>
+      <c r="C68">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A67*brute_life_multiplier</f>
+        <v>3528999851822864.5</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="6"/>
+        <v>235266656788190.97</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="7"/>
+        <v>2352666567882</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="8"/>
+        <v>117633328394095.48</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="9"/>
+        <v>4705333135764</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A68</f>
+        <v>364663318021696</v>
+      </c>
+      <c r="C69">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A68*brute_life_multiplier</f>
+        <v>5469949770325440</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>364663318021696</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="7"/>
+        <v>3646633180217</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="8"/>
+        <v>182331659010848</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="9"/>
+        <v>7293266360434</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A69</f>
+        <v>565228142933628.75</v>
+      </c>
+      <c r="C70">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A69*brute_life_multiplier</f>
+        <v>8478422144004431</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>565228142933628.75</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="7"/>
+        <v>5652281429337</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="8"/>
+        <v>282614071466814.38</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="9"/>
+        <v>11304562858673</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A70</f>
+        <v>876103621547124.75</v>
+      </c>
+      <c r="C71">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A70*brute_life_multiplier</f>
+        <v>1.3141554323206872E+16</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>876103621547124.75</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="7"/>
+        <v>8761036215472</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="8"/>
+        <v>438051810773562.38</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="9"/>
+        <v>17522072430943</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A71</f>
+        <v>1357960613398043.3</v>
+      </c>
+      <c r="C72">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A71*brute_life_multiplier</f>
+        <v>2.0369409200970648E+16</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>1357960613398043.3</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="7"/>
+        <v>13579606133981</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="8"/>
+        <v>678980306699021.63</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="9"/>
+        <v>27159212267961</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A72</f>
+        <v>2104838950766967.5</v>
+      </c>
+      <c r="C73">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A72*brute_life_multiplier</f>
+        <v>3.1572584261504512E+16</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>2104838950766967.5</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="7"/>
+        <v>21048389507670</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="8"/>
+        <v>1052419475383483.8</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="9"/>
+        <v>42096779015340</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A73</f>
+        <v>3262500373688800</v>
+      </c>
+      <c r="C74">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A73*brute_life_multiplier</f>
+        <v>4.8937505605332E+16</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>3262500373688800</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="7"/>
+        <v>32625003736888</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="8"/>
+        <v>1631250186844400</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="9"/>
+        <v>65250007473776</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A74</f>
+        <v>5056875579217641</v>
+      </c>
+      <c r="C75">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A74*brute_life_multiplier</f>
+        <v>7.5853133688264608E+16</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>5056875579217641</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="7"/>
+        <v>50568755792177</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="8"/>
+        <v>2528437789608820.5</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="9"/>
+        <v>101137511584353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A75</f>
+        <v>7838157147787344</v>
+      </c>
+      <c r="C76">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A75*brute_life_multiplier</f>
+        <v>1.1757235721681016E+17</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>7838157147787344</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="7"/>
+        <v>78381571477874</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="8"/>
+        <v>3919078573893672</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="9"/>
+        <v>156763142955747</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A76</f>
+        <v>1.2149143579070382E+16</v>
+      </c>
+      <c r="C77">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A76*brute_life_multiplier</f>
+        <v>1.8223715368605574E+17</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>1.2149143579070382E+16</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="7"/>
+        <v>121491435790704</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="8"/>
+        <v>6074571789535191</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="9"/>
+        <v>242982871581408</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A77</f>
+        <v>1.8831172547559092E+16</v>
+      </c>
+      <c r="C78">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A77*brute_life_multiplier</f>
+        <v>2.8246758821338637E+17</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>1.8831172547559092E+16</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="7"/>
+        <v>188311725475591</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="8"/>
+        <v>9415586273779546</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="9"/>
+        <v>376623450951182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A78</f>
+        <v>2.91883174487166E+16</v>
+      </c>
+      <c r="C79">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A78*brute_life_multiplier</f>
+        <v>4.3782476173074899E+17</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>2.91883174487166E+16</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="7"/>
+        <v>291883174487166</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="8"/>
+        <v>1.45941587243583E+16</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="9"/>
+        <v>583766348974332</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A79</f>
+        <v>4.5241892045510728E+16</v>
+      </c>
+      <c r="C80">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A79*brute_life_multiplier</f>
+        <v>6.7862838068266086E+17</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>4.5241892045510728E+16</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="7"/>
+        <v>452418920455107</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="8"/>
+        <v>2.2620946022755364E+16</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="9"/>
+        <v>904837840910215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A80</f>
+        <v>7.012493267054164E+16</v>
+      </c>
+      <c r="C81">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A80*brute_life_multiplier</f>
+        <v>1.0518739900581245E+18</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>7.012493267054164E+16</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="7"/>
+        <v>701249326705416</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="8"/>
+        <v>3.506246633527082E+16</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="9"/>
+        <v>1402498653410830</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A81</f>
+        <v>1.0869364563933955E+17</v>
+      </c>
+      <c r="C82">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A81*brute_life_multiplier</f>
+        <v>1.6304046845900933E+18</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>1.0869364563933955E+17</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="7"/>
+        <v>1086936456393400</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="8"/>
+        <v>5.4346822819669776E+16</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="9"/>
+        <v>2173872912786790</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A82</f>
+        <v>1.6847515074097629E+17</v>
+      </c>
+      <c r="C83">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A82*brute_life_multiplier</f>
+        <v>2.5271272611146445E+18</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>1.6847515074097629E+17</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="7"/>
+        <v>1684751507409760</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="8"/>
+        <v>8.4237575370488144E+16</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="9"/>
+        <v>3369503014819530</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A83</f>
+        <v>2.6113648364851325E+17</v>
+      </c>
+      <c r="C84">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A83*brute_life_multiplier</f>
+        <v>3.9170472547276989E+18</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>2.6113648364851325E+17</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="7"/>
+        <v>2611364836485130</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="8"/>
+        <v>1.3056824182425662E+17</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="9"/>
+        <v>5222729672970270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A84</f>
+        <v>4.0476154965519558E+17</v>
+      </c>
+      <c r="C85">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A84*brute_life_multiplier</f>
+        <v>6.0714232448279337E+18</v>
+      </c>
+      <c r="E85">
+        <f t="shared" ref="E85:E102" si="10" xml:space="preserve"> base_damage * hits_1_round_behind ^ A84</f>
+        <v>4.0476154965519558E+17</v>
+      </c>
+      <c r="F85">
+        <f t="shared" ref="F85:F102" si="11">ROUNDUP(B85/base_damage, 0)</f>
+        <v>4047615496551960</v>
+      </c>
+      <c r="G85">
+        <f t="shared" ref="G85:G102" si="12">E85/2</f>
+        <v>2.0238077482759779E+17</v>
+      </c>
+      <c r="H85">
+        <f t="shared" ref="H85:H102" si="13">ROUNDUP(B85/explosion_shot_base, 0)</f>
+        <v>8095230993103910</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A85</f>
+        <v>6.2738040196555315E+17</v>
+      </c>
+      <c r="C86">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A85*brute_life_multiplier</f>
+        <v>9.4107060294832968E+18</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="10"/>
+        <v>6.2738040196555315E+17</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="11"/>
+        <v>6273804019655530</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="12"/>
+        <v>3.1369020098277658E+17</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="13"/>
+        <v>1.25476080393111E+16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A86</f>
+        <v>9.7243962304660762E+17</v>
+      </c>
+      <c r="C87">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A86*brute_life_multiplier</f>
+        <v>1.4586594345699115E+19</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="10"/>
+        <v>9.7243962304660762E+17</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="11"/>
+        <v>9724396230466080</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="12"/>
+        <v>4.8621981152330381E+17</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="13"/>
+        <v>1.94487924609322E+16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A87</f>
+        <v>1.5072814157222418E+18</v>
+      </c>
+      <c r="C88">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A87*brute_life_multiplier</f>
+        <v>2.2609221235833627E+19</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="10"/>
+        <v>1.5072814157222418E+18</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="11"/>
+        <v>1.50728141572224E+16</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="12"/>
+        <v>7.536407078611209E+17</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="13"/>
+        <v>3.01456283144448E+16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A88</f>
+        <v>2.3362861943694751E+18</v>
+      </c>
+      <c r="C89">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A88*brute_life_multiplier</f>
+        <v>3.5044292915542127E+19</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="10"/>
+        <v>2.3362861943694751E+18</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="11"/>
+        <v>2.33628619436948E+16</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="12"/>
+        <v>1.1681430971847375E+18</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="13"/>
+        <v>4.6725723887389504E+16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A89</f>
+        <v>3.6212436012726866E+18</v>
+      </c>
+      <c r="C90">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A89*brute_life_multiplier</f>
+        <v>5.4318654019090301E+19</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="10"/>
+        <v>3.6212436012726866E+18</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="11"/>
+        <v>3.6212436012726896E+16</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="12"/>
+        <v>1.8106218006363433E+18</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="13"/>
+        <v>7.2424872025453696E+16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A90</f>
+        <v>5.6129275819726643E+18</v>
+      </c>
+      <c r="C91">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A90*brute_life_multiplier</f>
+        <v>8.4193913729589969E+19</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="10"/>
+        <v>5.6129275819726643E+18</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="11"/>
+        <v>5.61292758197266E+16</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="12"/>
+        <v>2.8064637909863322E+18</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="13"/>
+        <v>1.1225855163945299E+17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A91</f>
+        <v>8.7000377520576317E+18</v>
+      </c>
+      <c r="C92">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A91*brute_life_multiplier</f>
+        <v>1.3050056628086448E+20</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="10"/>
+        <v>8.7000377520576317E+18</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="11"/>
+        <v>8.7000377520576304E+16</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="12"/>
+        <v>4.3500188760288159E+18</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="13"/>
+        <v>1.7400075504115299E+17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A92</f>
+        <v>1.3485058515689329E+19</v>
+      </c>
+      <c r="C93">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A92*brute_life_multiplier</f>
+        <v>2.0227587773533992E+20</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="10"/>
+        <v>1.3485058515689329E+19</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="11"/>
+        <v>1.3485058515689299E+17</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="12"/>
+        <v>6.7425292578446643E+18</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="13"/>
+        <v>2.6970117031378701E+17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A93</f>
+        <v>2.0901840699318456E+19</v>
+      </c>
+      <c r="C94">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A93*brute_life_multiplier</f>
+        <v>3.1352761048977683E+20</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="10"/>
+        <v>2.0901840699318456E+19</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="11"/>
+        <v>2.0901840699318499E+17</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="12"/>
+        <v>1.0450920349659228E+19</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="13"/>
+        <v>4.1803681398636902E+17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A94</f>
+        <v>3.2397853083943617E+19</v>
+      </c>
+      <c r="C95">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A94*brute_life_multiplier</f>
+        <v>4.8596779625915423E+20</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="10"/>
+        <v>3.2397853083943617E+19</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="11"/>
+        <v>3.2397853083943603E+17</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="12"/>
+        <v>1.6198926541971808E+19</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="13"/>
+        <v>6.4795706167887206E+17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A95</f>
+        <v>5.0216672280112611E+19</v>
+      </c>
+      <c r="C96">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A95*brute_life_multiplier</f>
+        <v>7.5325008420168912E+20</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="10"/>
+        <v>5.0216672280112611E+19</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="11"/>
+        <v>5.0216672280112602E+17</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="12"/>
+        <v>2.5108336140056306E+19</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="13"/>
+        <v>1.00433344560225E+18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A96</f>
+        <v>7.7835842034174558E+19</v>
+      </c>
+      <c r="C97">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A96*brute_life_multiplier</f>
+        <v>1.1675376305126184E+21</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="10"/>
+        <v>7.7835842034174558E+19</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="11"/>
+        <v>7.7835842034174605E+17</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="12"/>
+        <v>3.8917921017087279E+19</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="13"/>
+        <v>1.55671684068349E+18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A97</f>
+        <v>1.2064555515297058E+20</v>
+      </c>
+      <c r="C98">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A97*brute_life_multiplier</f>
+        <v>1.8096833272945587E+21</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="10"/>
+        <v>1.2064555515297058E+20</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="11"/>
+        <v>1.2064555515297101E+18</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="12"/>
+        <v>6.032277757648529E+19</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="13"/>
+        <v>2.4129111030594099E+18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A98</f>
+        <v>1.8700061048710437E+20</v>
+      </c>
+      <c r="C99">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A98*brute_life_multiplier</f>
+        <v>2.8050091573065658E+21</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="10"/>
+        <v>1.8700061048710437E+20</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="11"/>
+        <v>1.87000610487104E+18</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="12"/>
+        <v>9.3500305243552186E+19</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="13"/>
+        <v>3.7400122097420902E+18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A99</f>
+        <v>2.8985094625501177E+20</v>
+      </c>
+      <c r="C100">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A99*brute_life_multiplier</f>
+        <v>4.3477641938251767E+21</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="10"/>
+        <v>2.8985094625501177E+20</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="11"/>
+        <v>2.8985094625501199E+18</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="12"/>
+        <v>1.4492547312750589E+20</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="13"/>
+        <v>5.7970189251002399E+18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A100</f>
+        <v>4.4926896669526832E+20</v>
+      </c>
+      <c r="C101">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A100*brute_life_multiplier</f>
+        <v>6.7390345004290251E+21</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="10"/>
+        <v>4.4926896669526832E+20</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="11"/>
+        <v>4.4926896669526799E+18</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="12"/>
+        <v>2.2463448334763416E+20</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="13"/>
+        <v>8.9853793339053701E+18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <f xml:space="preserve"> $B$3 * hits_1_round_behind ^ A101</f>
+        <v>6.9636689837766594E+20</v>
+      </c>
+      <c r="C102">
+        <f xml:space="preserve"> $B$3*hits_1_round_behind^A101*brute_life_multiplier</f>
+        <v>1.0445503475664988E+22</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="10"/>
+        <v>6.9636689837766594E+20</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="11"/>
+        <v>6.9636689837766605E+18</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="12"/>
+        <v>3.4818344918883297E+20</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="13"/>
+        <v>1.39273379675533E+19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weapons now scale as in excel
</commit_message>
<xml_diff>
--- a/docs/Balance/Balance.xlsx
+++ b/docs/Balance/Balance.xlsx
@@ -19,9 +19,9 @@
   </sheets>
   <definedNames>
     <definedName name="base_damage">Hoja1!$E$3</definedName>
-    <definedName name="brute_life_multiplier">Hoja1!$M$2</definedName>
-    <definedName name="explosion_shot_base">Hoja1!$G$3</definedName>
-    <definedName name="hits_1_round_behind">Hoja1!$M$1</definedName>
+    <definedName name="brute_life_multiplier">Hoja1!$O$2</definedName>
+    <definedName name="explosion_shot_base">Hoja1!$I$3</definedName>
+    <definedName name="hits_1_round_behind">Hoja1!$O$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>round</t>
-  </si>
-  <si>
-    <t>hits with weapon level 1</t>
   </si>
   <si>
     <t>hits to kill 1 round behind</t>
@@ -140,6 +137,15 @@
   </si>
   <si>
     <t>brute</t>
+  </si>
+  <si>
+    <t>hits level 1</t>
+  </si>
+  <si>
+    <t>hits level 2</t>
+  </si>
+  <si>
+    <t>hits level 3</t>
   </si>
 </sst>
 </file>
@@ -1087,13 +1093,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1381,89 +1387,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R102"/>
+  <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1">
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1">
         <v>1.55</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
+      <c r="G2" t="s">
+        <v>32</v>
       </c>
       <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2">
-        <v>15</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" t="str">
+      <c r="R2" t="str">
         <f>E2</f>
         <v>average weapon</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2">
+      <c r="S2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1480,32 +1494,40 @@
         <v>100</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F34" si="0">ROUNDUP(B3/base_damage, 0)</f>
+        <f>ROUNDUP(B3/base_damage, 0)</f>
         <v>1</v>
       </c>
       <c r="G3">
+        <f>ROUNDUP(B3/$E$4, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>ROUNDUP(B3/$E$5, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="I3">
         <f>base_damage/2</f>
         <v>50</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H34" si="1">ROUNDUP(B3/explosion_shot_base, 0)</f>
+      <c r="J3">
+        <f>ROUNDUP(B3/explosion_shot_base, 0)</f>
         <v>2</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" t="str">
+      <c r="Q3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="str">
         <f>B2</f>
         <v>tesla trooper</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3">
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1522,29 +1544,37 @@
         <v>155</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F4:F34" si="0">ROUNDUP(B4/base_damage, 0)</f>
         <v>2</v>
       </c>
       <c r="G4">
+        <f t="shared" ref="G4:G67" si="1">ROUNDUP(B4/$E$4, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H67" si="2">ROUNDUP(B4/$E$5, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="I4">
         <f>E4/2</f>
         <v>77.5</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
+      <c r="J4">
+        <f t="shared" ref="J4:J34" si="3">ROUNDUP(B4/explosion_shot_base, 0)</f>
         <v>4</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" t="str">
+        <f ca="1">OFFSET(R2,1, 0)</f>
+        <v>tesla trooper</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P4" t="str">
-        <f ca="1">OFFSET(P2,1, 0)</f>
-        <v>tesla trooper</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1565,16 +1595,24 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G61" si="2">E5/2</f>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I61" si="4">E5/2</f>
         <v>120.12500000000001</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
+      <c r="J5">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1595,15 +1633,23 @@
         <v>4</v>
       </c>
       <c r="G6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
         <v>186.19375000000002</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
+      <c r="J6">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1624,15 +1670,23 @@
         <v>6</v>
       </c>
       <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
         <v>288.60031250000009</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
+      <c r="J7">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1653,15 +1707,23 @@
         <v>9</v>
       </c>
       <c r="G8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
         <v>447.33048437500014</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1682,15 +1744,23 @@
         <v>14</v>
       </c>
       <c r="G9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
         <v>693.36225078125028</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1711,15 +1781,23 @@
         <v>22</v>
       </c>
       <c r="G10">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
         <v>1074.7114887109381</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
+      <c r="J10">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1740,15 +1818,23 @@
         <v>34</v>
       </c>
       <c r="G11">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
         <v>1665.802807501954</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
+      <c r="J11">
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1769,15 +1855,23 @@
         <v>52</v>
       </c>
       <c r="G12">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
         <v>2581.9943516280291</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
+      <c r="J12">
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1798,15 +1892,23 @@
         <v>81</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
         <v>4002.0912450234446</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
+      <c r="J13">
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1827,15 +1929,23 @@
         <v>125</v>
       </c>
       <c r="G14">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
         <v>6203.2414297863397</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
+      <c r="J14">
+        <f t="shared" si="3"/>
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1856,15 +1966,23 @@
         <v>193</v>
       </c>
       <c r="G15">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
         <v>9615.0242161688275</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
+      <c r="J15">
+        <f t="shared" si="3"/>
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1885,15 +2003,23 @@
         <v>299</v>
       </c>
       <c r="G16">
+        <f t="shared" si="1"/>
+        <v>193</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
         <v>14903.287535061685</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
+      <c r="J16">
+        <f t="shared" si="3"/>
         <v>597</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1914,15 +2040,23 @@
         <v>463</v>
       </c>
       <c r="G17">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
         <v>23100.095679345613</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
+      <c r="J17">
+        <f t="shared" si="3"/>
         <v>925</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1943,15 +2077,23 @@
         <v>717</v>
       </c>
       <c r="G18">
+        <f t="shared" si="1"/>
+        <v>463</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="2"/>
+        <v>299</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
         <v>35805.148302985705</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
+      <c r="J18">
+        <f t="shared" si="3"/>
         <v>1433</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1972,15 +2114,23 @@
         <v>1110</v>
       </c>
       <c r="G19">
+        <f t="shared" si="1"/>
+        <v>717</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="2"/>
+        <v>463</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
         <v>55497.979869627838</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
+      <c r="J19">
+        <f t="shared" si="3"/>
         <v>2220</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2001,15 +2151,23 @@
         <v>1721</v>
       </c>
       <c r="G20">
+        <f t="shared" si="1"/>
+        <v>1110</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="2"/>
+        <v>717</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
         <v>86021.868797923147</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
+      <c r="J20">
+        <f t="shared" si="3"/>
         <v>3441</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2030,15 +2188,23 @@
         <v>2667</v>
       </c>
       <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1721</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
         <v>133333.8966367809</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
+      <c r="J21">
+        <f t="shared" si="3"/>
         <v>5334</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2059,15 +2225,23 @@
         <v>4134</v>
       </c>
       <c r="G22">
+        <f t="shared" si="1"/>
+        <v>2667</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
+        <v>1721</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
         <v>206667.53978701041</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
+      <c r="J22">
+        <f t="shared" si="3"/>
         <v>8267</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2088,15 +2262,23 @@
         <v>6407</v>
       </c>
       <c r="G23">
+        <f t="shared" si="1"/>
+        <v>4134</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="2"/>
+        <v>2667</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
         <v>320334.68666986615</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
+      <c r="J23">
+        <f t="shared" si="3"/>
         <v>12814</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2117,15 +2299,23 @@
         <v>9931</v>
       </c>
       <c r="G24">
+        <f t="shared" si="1"/>
+        <v>6407</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
+        <v>4134</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
         <v>496518.76433829259</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
+      <c r="J24">
+        <f t="shared" si="3"/>
         <v>19861</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2146,15 +2336,23 @@
         <v>15393</v>
       </c>
       <c r="G25">
+        <f t="shared" si="1"/>
+        <v>9931</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
+        <v>6407</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
         <v>769604.08472435351</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
+      <c r="J25">
+        <f t="shared" si="3"/>
         <v>30785</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2175,15 +2373,23 @@
         <v>23858</v>
       </c>
       <c r="G26">
+        <f t="shared" si="1"/>
+        <v>15393</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
+        <v>9931</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
         <v>1192886.331322748</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="1"/>
+      <c r="J26">
+        <f t="shared" si="3"/>
         <v>47716</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2204,15 +2410,23 @@
         <v>36980</v>
       </c>
       <c r="G27">
+        <f t="shared" si="1"/>
+        <v>23858</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
+        <v>15393</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
         <v>1848973.8135502597</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="1"/>
+      <c r="J27">
+        <f t="shared" si="3"/>
         <v>73959</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2233,15 +2447,23 @@
         <v>57319</v>
       </c>
       <c r="G28">
+        <f t="shared" si="1"/>
+        <v>36980</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
+        <v>23858</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
         <v>2865909.4110029028</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
+      <c r="J28">
+        <f t="shared" si="3"/>
         <v>114637</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2262,15 +2484,23 @@
         <v>88844</v>
       </c>
       <c r="G29">
+        <f t="shared" si="1"/>
+        <v>57319</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
+        <v>36980</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
         <v>4442159.5870544994</v>
       </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
+      <c r="J29">
+        <f t="shared" si="3"/>
         <v>177687</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2291,15 +2521,23 @@
         <v>137707</v>
       </c>
       <c r="G30">
+        <f t="shared" si="1"/>
+        <v>88844</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="2"/>
+        <v>57319</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="4"/>
         <v>6885347.3599344743</v>
       </c>
-      <c r="H30">
-        <f t="shared" si="1"/>
+      <c r="J30">
+        <f t="shared" si="3"/>
         <v>275414</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2320,15 +2558,23 @@
         <v>213446</v>
       </c>
       <c r="G31">
+        <f t="shared" si="1"/>
+        <v>137707</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="2"/>
+        <v>88844</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
         <v>10672288.407898437</v>
       </c>
-      <c r="H31">
-        <f t="shared" si="1"/>
+      <c r="J31">
+        <f t="shared" si="3"/>
         <v>426892</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2349,15 +2595,23 @@
         <v>330841</v>
       </c>
       <c r="G32">
+        <f t="shared" si="1"/>
+        <v>213446</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="2"/>
+        <v>137707</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
         <v>16542047.032242578</v>
       </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
+      <c r="J32">
+        <f t="shared" si="3"/>
         <v>661682</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2378,15 +2632,23 @@
         <v>512804</v>
       </c>
       <c r="G33">
+        <f t="shared" si="1"/>
+        <v>330841</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="2"/>
+        <v>213446</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="4"/>
         <v>25640172.899976</v>
       </c>
-      <c r="H33">
-        <f t="shared" si="1"/>
+      <c r="J33">
+        <f t="shared" si="3"/>
         <v>1025607</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2407,15 +2669,23 @@
         <v>794846</v>
       </c>
       <c r="G34">
+        <f t="shared" si="1"/>
+        <v>512804</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="2"/>
+        <v>330841</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
         <v>39742267.994962804</v>
       </c>
-      <c r="H34">
-        <f t="shared" si="1"/>
+      <c r="J34">
+        <f t="shared" si="3"/>
         <v>1589691</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2432,19 +2702,27 @@
         <v>123201030.78438467</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F61" si="3">ROUNDUP(B35/base_damage, 0)</f>
+        <f t="shared" ref="F35:F61" si="5">ROUNDUP(B35/base_damage, 0)</f>
         <v>1232011</v>
       </c>
       <c r="G35">
+        <f t="shared" si="1"/>
+        <v>794846</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="2"/>
+        <v>512804</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
         <v>61600515.392192334</v>
       </c>
-      <c r="H35">
-        <f t="shared" ref="H35:H61" si="4">ROUNDUP(B35/explosion_shot_base, 0)</f>
+      <c r="J35">
+        <f t="shared" ref="J35:J61" si="6">ROUNDUP(B35/explosion_shot_base, 0)</f>
         <v>2464021</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2457,23 +2735,31 @@
         <v>2864423965.7369437</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:E61" si="5" xml:space="preserve"> base_damage * hits_1_round_behind ^ A35</f>
+        <f t="shared" ref="E36:E61" si="7" xml:space="preserve"> base_damage * hits_1_round_behind ^ A35</f>
         <v>190961597.71579626</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1909616</v>
       </c>
       <c r="G36">
+        <f t="shared" si="1"/>
+        <v>1232011</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="2"/>
+        <v>794846</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
         <v>95480798.857898131</v>
       </c>
-      <c r="H36">
-        <f t="shared" si="4"/>
+      <c r="J36">
+        <f t="shared" si="6"/>
         <v>3819232</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2486,23 +2772,31 @@
         <v>4439857146.8922634</v>
       </c>
       <c r="E37">
+        <f t="shared" si="7"/>
+        <v>295990476.45948422</v>
+      </c>
+      <c r="F37">
         <f t="shared" si="5"/>
-        <v>295990476.45948422</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="3"/>
         <v>2959905</v>
       </c>
       <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1909616</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="2"/>
+        <v>1232011</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
         <v>147995238.22974211</v>
       </c>
-      <c r="H37">
-        <f t="shared" si="4"/>
+      <c r="J37">
+        <f t="shared" si="6"/>
         <v>5919810</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2515,23 +2809,31 @@
         <v>6881778577.6830091</v>
       </c>
       <c r="E38">
+        <f t="shared" si="7"/>
+        <v>458785238.51220059</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="5"/>
-        <v>458785238.51220059</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="3"/>
         <v>4587853</v>
       </c>
       <c r="G38">
+        <f t="shared" si="1"/>
+        <v>2959905</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="2"/>
+        <v>1909616</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
         <v>229392619.2561003</v>
       </c>
-      <c r="H38">
-        <f t="shared" si="4"/>
+      <c r="J38">
+        <f t="shared" si="6"/>
         <v>9175705</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2544,23 +2846,31 @@
         <v>10666756795.408663</v>
       </c>
       <c r="E39">
+        <f t="shared" si="7"/>
+        <v>711117119.69391084</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="5"/>
-        <v>711117119.69391084</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="3"/>
         <v>7111172</v>
       </c>
       <c r="G39">
+        <f t="shared" si="1"/>
+        <v>4587853</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="2"/>
+        <v>2959905</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
         <v>355558559.84695542</v>
       </c>
-      <c r="H39">
-        <f t="shared" si="4"/>
+      <c r="J39">
+        <f t="shared" si="6"/>
         <v>14222343</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2573,23 +2883,31 @@
         <v>16533473032.883427</v>
       </c>
       <c r="E40">
+        <f t="shared" si="7"/>
+        <v>1102231535.5255618</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="5"/>
-        <v>1102231535.5255618</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="3"/>
         <v>11022316</v>
       </c>
       <c r="G40">
+        <f t="shared" si="1"/>
+        <v>7111172</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="2"/>
+        <v>4587853</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
         <v>551115767.7627809</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="4"/>
+      <c r="J40">
+        <f t="shared" si="6"/>
         <v>22044631</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2602,23 +2920,31 @@
         <v>25626883200.969318</v>
       </c>
       <c r="E41">
+        <f t="shared" si="7"/>
+        <v>1708458880.0646212</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="5"/>
-        <v>1708458880.0646212</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="3"/>
         <v>17084589</v>
       </c>
       <c r="G41">
+        <f t="shared" si="1"/>
+        <v>11022316</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="2"/>
+        <v>7111172</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
         <v>854229440.03231061</v>
       </c>
-      <c r="H41">
-        <f t="shared" si="4"/>
+      <c r="J41">
+        <f t="shared" si="6"/>
         <v>34169178</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2631,23 +2957,31 @@
         <v>39721668961.502441</v>
       </c>
       <c r="E42">
+        <f t="shared" si="7"/>
+        <v>2648111264.100163</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="5"/>
-        <v>2648111264.100163</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="3"/>
         <v>26481113</v>
       </c>
       <c r="G42">
+        <f t="shared" si="1"/>
+        <v>17084589</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="2"/>
+        <v>11022316</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="4"/>
         <v>1324055632.0500815</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="4"/>
+      <c r="J42">
+        <f t="shared" si="6"/>
         <v>52962226</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2660,23 +2994,31 @@
         <v>61568586890.328796</v>
       </c>
       <c r="E43">
+        <f t="shared" si="7"/>
+        <v>4104572459.3552532</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="5"/>
-        <v>4104572459.3552532</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="3"/>
         <v>41045725</v>
       </c>
       <c r="G43">
+        <f t="shared" si="1"/>
+        <v>26481113</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="2"/>
+        <v>17084589</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="4"/>
         <v>2052286229.6776266</v>
       </c>
-      <c r="H43">
-        <f t="shared" si="4"/>
+      <c r="J43">
+        <f t="shared" si="6"/>
         <v>82091450</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2689,23 +3031,31 @@
         <v>95431309680.009644</v>
       </c>
       <c r="E44">
+        <f t="shared" si="7"/>
+        <v>6362087312.0006428</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="5"/>
-        <v>6362087312.0006428</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="3"/>
         <v>63620874</v>
       </c>
       <c r="G44">
+        <f t="shared" si="1"/>
+        <v>41045725</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="2"/>
+        <v>26481113</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="4"/>
         <v>3181043656.0003214</v>
       </c>
-      <c r="H44">
-        <f t="shared" si="4"/>
+      <c r="J44">
+        <f t="shared" si="6"/>
         <v>127241747</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2718,23 +3068,31 @@
         <v>147918530004.01495</v>
       </c>
       <c r="E45">
+        <f t="shared" si="7"/>
+        <v>9861235333.600996</v>
+      </c>
+      <c r="F45">
         <f t="shared" si="5"/>
-        <v>9861235333.600996</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="3"/>
         <v>98612354</v>
       </c>
       <c r="G45">
+        <f t="shared" si="1"/>
+        <v>63620874</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="2"/>
+        <v>41045725</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
         <v>4930617666.800498</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="4"/>
+      <c r="J45">
+        <f t="shared" si="6"/>
         <v>197224707</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2747,23 +3105,31 @@
         <v>229273721506.22314</v>
       </c>
       <c r="E46">
+        <f t="shared" si="7"/>
+        <v>15284914767.081543</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="5"/>
-        <v>15284914767.081543</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="3"/>
         <v>152849148</v>
       </c>
       <c r="G46">
+        <f t="shared" si="1"/>
+        <v>98612354</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="2"/>
+        <v>63620874</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
         <v>7642457383.5407715</v>
       </c>
-      <c r="H46">
-        <f t="shared" si="4"/>
+      <c r="J46">
+        <f t="shared" si="6"/>
         <v>305698296</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2776,23 +3142,31 @@
         <v>355374268334.646</v>
       </c>
       <c r="E47">
+        <f t="shared" si="7"/>
+        <v>23691617888.976398</v>
+      </c>
+      <c r="F47">
         <f t="shared" si="5"/>
-        <v>23691617888.976398</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="3"/>
         <v>236916179</v>
       </c>
       <c r="G47">
+        <f t="shared" si="1"/>
+        <v>152849148</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="2"/>
+        <v>98612354</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="4"/>
         <v>11845808944.488199</v>
       </c>
-      <c r="H47">
-        <f t="shared" si="4"/>
+      <c r="J47">
+        <f t="shared" si="6"/>
         <v>473832358</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2805,23 +3179,31 @@
         <v>550830115918.70129</v>
       </c>
       <c r="E48">
+        <f t="shared" si="7"/>
+        <v>36722007727.913422</v>
+      </c>
+      <c r="F48">
         <f t="shared" si="5"/>
-        <v>36722007727.913422</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="3"/>
         <v>367220078</v>
       </c>
       <c r="G48">
+        <f t="shared" si="1"/>
+        <v>236916179</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="2"/>
+        <v>152849148</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="4"/>
         <v>18361003863.956711</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="4"/>
+      <c r="J48">
+        <f t="shared" si="6"/>
         <v>734440155</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2834,23 +3216,31 @@
         <v>853786679673.98706</v>
       </c>
       <c r="E49">
+        <f t="shared" si="7"/>
+        <v>56919111978.265808</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="5"/>
-        <v>56919111978.265808</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="3"/>
         <v>569191120</v>
       </c>
       <c r="G49">
+        <f t="shared" si="1"/>
+        <v>367220078</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="2"/>
+        <v>236916179</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="4"/>
         <v>28459555989.132904</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="4"/>
+      <c r="J49">
+        <f t="shared" si="6"/>
         <v>1138382240</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2863,23 +3253,31 @@
         <v>1323369353494.6799</v>
       </c>
       <c r="E50">
+        <f t="shared" si="7"/>
+        <v>88224623566.311996</v>
+      </c>
+      <c r="F50">
         <f t="shared" si="5"/>
-        <v>88224623566.311996</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="3"/>
         <v>882246236</v>
       </c>
       <c r="G50">
+        <f t="shared" si="1"/>
+        <v>569191120</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="2"/>
+        <v>367220078</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="4"/>
         <v>44112311783.155998</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="4"/>
+      <c r="J50">
+        <f t="shared" si="6"/>
         <v>1764492472</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2892,23 +3290,31 @@
         <v>2051222497916.7542</v>
       </c>
       <c r="E51">
+        <f t="shared" si="7"/>
+        <v>136748166527.78362</v>
+      </c>
+      <c r="F51">
         <f t="shared" si="5"/>
-        <v>136748166527.78362</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="3"/>
         <v>1367481666</v>
       </c>
       <c r="G51">
+        <f t="shared" si="1"/>
+        <v>882246236</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="2"/>
+        <v>569191120</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="4"/>
         <v>68374083263.891808</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="4"/>
+      <c r="J51">
+        <f t="shared" si="6"/>
         <v>2734963331</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2921,23 +3327,31 @@
         <v>3179394871770.9692</v>
       </c>
       <c r="E52">
+        <f t="shared" si="7"/>
+        <v>211959658118.06461</v>
+      </c>
+      <c r="F52">
         <f t="shared" si="5"/>
-        <v>211959658118.06461</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="3"/>
         <v>2119596582</v>
       </c>
       <c r="G52">
+        <f t="shared" si="1"/>
+        <v>1367481666</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="2"/>
+        <v>882246236</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="4"/>
         <v>105979829059.0323</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="4"/>
+      <c r="J52">
+        <f t="shared" si="6"/>
         <v>4239193163</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2950,23 +3364,31 @@
         <v>4928062051245.002</v>
       </c>
       <c r="E53">
+        <f t="shared" si="7"/>
+        <v>328537470083.00012</v>
+      </c>
+      <c r="F53">
         <f t="shared" si="5"/>
-        <v>328537470083.00012</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="3"/>
         <v>3285374701</v>
       </c>
       <c r="G53">
+        <f t="shared" si="1"/>
+        <v>2119596582</v>
+      </c>
+      <c r="H53">
         <f t="shared" si="2"/>
+        <v>1367481666</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="4"/>
         <v>164268735041.50006</v>
       </c>
-      <c r="H53">
-        <f t="shared" si="4"/>
+      <c r="J53">
+        <f t="shared" si="6"/>
         <v>6570749402</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2979,23 +3401,31 @@
         <v>7638496179429.7539</v>
       </c>
       <c r="E54">
+        <f t="shared" si="7"/>
+        <v>509233078628.65027</v>
+      </c>
+      <c r="F54">
         <f t="shared" si="5"/>
-        <v>509233078628.65027</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="3"/>
         <v>5092330787</v>
       </c>
       <c r="G54">
+        <f t="shared" si="1"/>
+        <v>3285374701</v>
+      </c>
+      <c r="H54">
         <f t="shared" si="2"/>
+        <v>2119596582</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="4"/>
         <v>254616539314.32513</v>
       </c>
-      <c r="H54">
-        <f t="shared" si="4"/>
+      <c r="J54">
+        <f t="shared" si="6"/>
         <v>10184661573</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3008,23 +3438,31 @@
         <v>11839669078116.119</v>
       </c>
       <c r="E55">
+        <f t="shared" si="7"/>
+        <v>789311271874.40796</v>
+      </c>
+      <c r="F55">
         <f t="shared" si="5"/>
-        <v>789311271874.40796</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="3"/>
         <v>7893112719</v>
       </c>
       <c r="G55">
+        <f t="shared" si="1"/>
+        <v>5092330787</v>
+      </c>
+      <c r="H55">
         <f t="shared" si="2"/>
+        <v>3285374701</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="4"/>
         <v>394655635937.20398</v>
       </c>
-      <c r="H55">
-        <f t="shared" si="4"/>
+      <c r="J55">
+        <f t="shared" si="6"/>
         <v>15786225438</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3037,23 +3475,31 @@
         <v>18351487071079.984</v>
       </c>
       <c r="E56">
+        <f t="shared" si="7"/>
+        <v>1223432471405.3323</v>
+      </c>
+      <c r="F56">
         <f t="shared" si="5"/>
-        <v>1223432471405.3323</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="3"/>
         <v>12234324715</v>
       </c>
       <c r="G56">
+        <f t="shared" si="1"/>
+        <v>7893112719</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="2"/>
+        <v>5092330787</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="4"/>
         <v>611716235702.66614</v>
       </c>
-      <c r="H56">
-        <f t="shared" si="4"/>
+      <c r="J56">
+        <f t="shared" si="6"/>
         <v>24468649429</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3066,23 +3512,31 @@
         <v>28444804960173.98</v>
       </c>
       <c r="E57">
+        <f t="shared" si="7"/>
+        <v>1896320330678.2654</v>
+      </c>
+      <c r="F57">
         <f t="shared" si="5"/>
-        <v>1896320330678.2654</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="3"/>
         <v>18963203307</v>
       </c>
       <c r="G57">
+        <f t="shared" si="1"/>
+        <v>12234324715</v>
+      </c>
+      <c r="H57">
         <f t="shared" si="2"/>
+        <v>7893112719</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="4"/>
         <v>948160165339.13269</v>
       </c>
-      <c r="H57">
-        <f t="shared" si="4"/>
+      <c r="J57">
+        <f t="shared" si="6"/>
         <v>37926406614</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3095,23 +3549,31 @@
         <v>44089447688269.672</v>
       </c>
       <c r="E58">
+        <f t="shared" si="7"/>
+        <v>2939296512551.3115</v>
+      </c>
+      <c r="F58">
         <f t="shared" si="5"/>
-        <v>2939296512551.3115</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="3"/>
         <v>29392965126</v>
       </c>
       <c r="G58">
+        <f t="shared" si="1"/>
+        <v>18963203307</v>
+      </c>
+      <c r="H58">
         <f t="shared" si="2"/>
+        <v>12234324715</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="4"/>
         <v>1469648256275.6558</v>
       </c>
-      <c r="H58">
-        <f t="shared" si="4"/>
+      <c r="J58">
+        <f t="shared" si="6"/>
         <v>58785930252</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3124,23 +3586,31 @@
         <v>68338643916818</v>
       </c>
       <c r="E59">
+        <f t="shared" si="7"/>
+        <v>4555909594454.5332</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="5"/>
-        <v>4555909594454.5332</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="3"/>
         <v>45559095945</v>
       </c>
       <c r="G59">
+        <f t="shared" si="1"/>
+        <v>29392965126</v>
+      </c>
+      <c r="H59">
         <f t="shared" si="2"/>
+        <v>18963203307</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="4"/>
         <v>2277954797227.2666</v>
       </c>
-      <c r="H59">
-        <f t="shared" si="4"/>
+      <c r="J59">
+        <f t="shared" si="6"/>
         <v>91118191890</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3153,23 +3623,31 @@
         <v>105924898071067.91</v>
       </c>
       <c r="E60">
+        <f t="shared" si="7"/>
+        <v>7061659871404.5273</v>
+      </c>
+      <c r="F60">
         <f t="shared" si="5"/>
-        <v>7061659871404.5273</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="3"/>
         <v>70616598715</v>
       </c>
       <c r="G60">
+        <f t="shared" si="1"/>
+        <v>45559095945</v>
+      </c>
+      <c r="H60">
         <f t="shared" si="2"/>
+        <v>29392965126</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="4"/>
         <v>3530829935702.2637</v>
       </c>
-      <c r="H60">
-        <f t="shared" si="4"/>
+      <c r="J60">
+        <f t="shared" si="6"/>
         <v>141233197429</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3182,23 +3660,31 @@
         <v>164183592010155.28</v>
       </c>
       <c r="E61">
+        <f t="shared" si="7"/>
+        <v>10945572800677.02</v>
+      </c>
+      <c r="F61">
         <f t="shared" si="5"/>
-        <v>10945572800677.02</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="3"/>
         <v>109455728007</v>
       </c>
       <c r="G61">
+        <f t="shared" si="1"/>
+        <v>70616598715</v>
+      </c>
+      <c r="H61">
         <f t="shared" si="2"/>
+        <v>45559095945</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="4"/>
         <v>5472786400338.5098</v>
       </c>
-      <c r="H61">
-        <f t="shared" si="4"/>
+      <c r="J61">
+        <f t="shared" si="6"/>
         <v>218911456014</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3211,23 +3697,31 @@
         <v>254484567615740.66</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:E84" si="6" xml:space="preserve"> base_damage * hits_1_round_behind ^ A61</f>
+        <f t="shared" ref="E62:E84" si="8" xml:space="preserve"> base_damage * hits_1_round_behind ^ A61</f>
         <v>16965637841049.377</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:F84" si="7">ROUNDUP(B62/base_damage, 0)</f>
+        <f t="shared" ref="F62:F84" si="9">ROUNDUP(B62/base_damage, 0)</f>
         <v>169656378411</v>
       </c>
       <c r="G62">
-        <f t="shared" ref="G62:G84" si="8">E62/2</f>
+        <f t="shared" si="1"/>
+        <v>109455728007</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>70616598715</v>
+      </c>
+      <c r="I62">
+        <f t="shared" ref="I62:I84" si="10">E62/2</f>
         <v>8482818920524.6885</v>
       </c>
-      <c r="H62">
-        <f t="shared" ref="H62:H84" si="9">ROUNDUP(B62/explosion_shot_base, 0)</f>
+      <c r="J62">
+        <f t="shared" ref="J62:J84" si="11">ROUNDUP(B62/explosion_shot_base, 0)</f>
         <v>339312756821</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3240,23 +3734,31 @@
         <v>394451079804398.13</v>
       </c>
       <c r="E63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>26296738653626.543</v>
       </c>
       <c r="F63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>262967386537</v>
       </c>
       <c r="G63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
+        <v>169656378411</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>109455728007</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="10"/>
         <v>13148369326813.271</v>
       </c>
-      <c r="H63">
-        <f t="shared" si="9"/>
+      <c r="J63">
+        <f t="shared" si="11"/>
         <v>525934773073</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3269,23 +3771,31 @@
         <v>611399173696817</v>
       </c>
       <c r="E64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>40759944913121.133</v>
       </c>
       <c r="F64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>407599449132</v>
       </c>
       <c r="G64">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
+        <v>262967386537</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>169656378411</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="10"/>
         <v>20379972456560.566</v>
       </c>
-      <c r="H64">
-        <f t="shared" si="9"/>
+      <c r="J64">
+        <f t="shared" si="11"/>
         <v>815198898263</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3298,23 +3808,31 @@
         <v>947668719230066.75</v>
       </c>
       <c r="E65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>63177914615337.781</v>
       </c>
       <c r="F65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>631779146154</v>
       </c>
       <c r="G65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
+        <v>407599449132</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>262967386537</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="10"/>
         <v>31588957307668.891</v>
       </c>
-      <c r="H65">
-        <f t="shared" si="9"/>
+      <c r="J65">
+        <f t="shared" si="11"/>
         <v>1263558292307</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3327,23 +3845,31 @@
         <v>1468886514806603.5</v>
       </c>
       <c r="E66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97925767653773.563</v>
       </c>
       <c r="F66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>979257676538</v>
       </c>
       <c r="G66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
+        <v>631779146154</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>407599449132</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="10"/>
         <v>48962883826886.781</v>
       </c>
-      <c r="H66">
-        <f t="shared" si="9"/>
+      <c r="J66">
+        <f t="shared" si="11"/>
         <v>1958515353076</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3356,23 +3882,31 @@
         <v>2276774097950235</v>
       </c>
       <c r="E67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>151784939863349</v>
       </c>
       <c r="F67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1517849398634</v>
       </c>
       <c r="G67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
+        <v>979257676538</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="2"/>
+        <v>631779146154</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="10"/>
         <v>75892469931674.5</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="9"/>
+      <c r="J67">
+        <f t="shared" si="11"/>
         <v>3035698797267</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3385,23 +3919,31 @@
         <v>3528999851822864.5</v>
       </c>
       <c r="E68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>235266656788190.97</v>
       </c>
       <c r="F68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2352666567882</v>
       </c>
       <c r="G68">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="G68:G92" si="12">ROUNDUP(B68/$E$4, 0)</f>
+        <v>1517849398634</v>
+      </c>
+      <c r="H68">
+        <f t="shared" ref="H68:H102" si="13">ROUNDUP(B68/$E$5, 0)</f>
+        <v>979257676538</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="10"/>
         <v>117633328394095.48</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="9"/>
+      <c r="J68">
+        <f t="shared" si="11"/>
         <v>4705333135764</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3414,23 +3956,31 @@
         <v>5469949770325440</v>
       </c>
       <c r="E69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>364663318021696</v>
       </c>
       <c r="F69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3646633180217</v>
       </c>
       <c r="G69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>2352666567882</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="13"/>
+        <v>1517849398634</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="10"/>
         <v>182331659010848</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="9"/>
+      <c r="J69">
+        <f t="shared" si="11"/>
         <v>7293266360434</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3443,23 +3993,31 @@
         <v>8478422144004431</v>
       </c>
       <c r="E70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>565228142933628.75</v>
       </c>
       <c r="F70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5652281429337</v>
       </c>
       <c r="G70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>3646633180217</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="13"/>
+        <v>2352666567882</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="10"/>
         <v>282614071466814.38</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="9"/>
+      <c r="J70">
+        <f t="shared" si="11"/>
         <v>11304562858673</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3472,23 +4030,31 @@
         <v>1.3141554323206872E+16</v>
       </c>
       <c r="E71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>876103621547124.75</v>
       </c>
       <c r="F71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8761036215472</v>
       </c>
       <c r="G71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>5652281429337</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="13"/>
+        <v>3646633180217</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="10"/>
         <v>438051810773562.38</v>
       </c>
-      <c r="H71">
-        <f t="shared" si="9"/>
+      <c r="J71">
+        <f t="shared" si="11"/>
         <v>17522072430943</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3501,23 +4067,31 @@
         <v>2.0369409200970648E+16</v>
       </c>
       <c r="E72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1357960613398043.3</v>
       </c>
       <c r="F72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13579606133981</v>
       </c>
       <c r="G72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>8761036215472</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="13"/>
+        <v>5652281429337</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="10"/>
         <v>678980306699021.63</v>
       </c>
-      <c r="H72">
-        <f t="shared" si="9"/>
+      <c r="J72">
+        <f t="shared" si="11"/>
         <v>27159212267961</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3530,23 +4104,31 @@
         <v>3.1572584261504512E+16</v>
       </c>
       <c r="E73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2104838950766967.5</v>
       </c>
       <c r="F73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>21048389507670</v>
       </c>
       <c r="G73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>13579606133981</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="13"/>
+        <v>8761036215472</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="10"/>
         <v>1052419475383483.8</v>
       </c>
-      <c r="H73">
-        <f t="shared" si="9"/>
+      <c r="J73">
+        <f t="shared" si="11"/>
         <v>42096779015340</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3559,23 +4141,31 @@
         <v>4.8937505605332E+16</v>
       </c>
       <c r="E74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3262500373688800</v>
       </c>
       <c r="F74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>32625003736888</v>
       </c>
       <c r="G74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>21048389507670</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="13"/>
+        <v>13579606133981</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="10"/>
         <v>1631250186844400</v>
       </c>
-      <c r="H74">
-        <f t="shared" si="9"/>
+      <c r="J74">
+        <f t="shared" si="11"/>
         <v>65250007473776</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3588,23 +4178,31 @@
         <v>7.5853133688264608E+16</v>
       </c>
       <c r="E75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5056875579217641</v>
       </c>
       <c r="F75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>50568755792177</v>
       </c>
       <c r="G75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>32625003736888</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="13"/>
+        <v>21048389507670</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="10"/>
         <v>2528437789608820.5</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="9"/>
+      <c r="J75">
+        <f t="shared" si="11"/>
         <v>101137511584353</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3617,23 +4215,31 @@
         <v>1.1757235721681016E+17</v>
       </c>
       <c r="E76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7838157147787344</v>
       </c>
       <c r="F76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>78381571477874</v>
       </c>
       <c r="G76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>50568755792177</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="13"/>
+        <v>32625003736888</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="10"/>
         <v>3919078573893672</v>
       </c>
-      <c r="H76">
-        <f t="shared" si="9"/>
+      <c r="J76">
+        <f t="shared" si="11"/>
         <v>156763142955747</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3646,23 +4252,31 @@
         <v>1.8223715368605574E+17</v>
       </c>
       <c r="E77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2149143579070382E+16</v>
       </c>
       <c r="F77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>121491435790704</v>
       </c>
       <c r="G77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>78381571477874</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="13"/>
+        <v>50568755792177</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="10"/>
         <v>6074571789535191</v>
       </c>
-      <c r="H77">
-        <f t="shared" si="9"/>
+      <c r="J77">
+        <f t="shared" si="11"/>
         <v>242982871581408</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3675,23 +4289,31 @@
         <v>2.8246758821338637E+17</v>
       </c>
       <c r="E78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.8831172547559092E+16</v>
       </c>
       <c r="F78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>188311725475591</v>
       </c>
       <c r="G78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>121491435790704</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="13"/>
+        <v>78381571477874</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="10"/>
         <v>9415586273779546</v>
       </c>
-      <c r="H78">
-        <f t="shared" si="9"/>
+      <c r="J78">
+        <f t="shared" si="11"/>
         <v>376623450951182</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3704,23 +4326,31 @@
         <v>4.3782476173074899E+17</v>
       </c>
       <c r="E79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.91883174487166E+16</v>
       </c>
       <c r="F79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>291883174487166</v>
       </c>
       <c r="G79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>188311725475591</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="13"/>
+        <v>121491435790704</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="10"/>
         <v>1.45941587243583E+16</v>
       </c>
-      <c r="H79">
-        <f t="shared" si="9"/>
+      <c r="J79">
+        <f t="shared" si="11"/>
         <v>583766348974332</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3733,23 +4363,31 @@
         <v>6.7862838068266086E+17</v>
       </c>
       <c r="E80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.5241892045510728E+16</v>
       </c>
       <c r="F80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>452418920455107</v>
       </c>
       <c r="G80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>291883174487166</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="13"/>
+        <v>188311725475591</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="10"/>
         <v>2.2620946022755364E+16</v>
       </c>
-      <c r="H80">
-        <f t="shared" si="9"/>
+      <c r="J80">
+        <f t="shared" si="11"/>
         <v>904837840910215</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3762,23 +4400,31 @@
         <v>1.0518739900581245E+18</v>
       </c>
       <c r="E81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.012493267054164E+16</v>
       </c>
       <c r="F81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>701249326705416</v>
       </c>
       <c r="G81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>452418920455107</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="13"/>
+        <v>291883174487166</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="10"/>
         <v>3.506246633527082E+16</v>
       </c>
-      <c r="H81">
-        <f t="shared" si="9"/>
+      <c r="J81">
+        <f t="shared" si="11"/>
         <v>1402498653410830</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3791,23 +4437,31 @@
         <v>1.6304046845900933E+18</v>
       </c>
       <c r="E82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0869364563933955E+17</v>
       </c>
       <c r="F82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1086936456393400</v>
       </c>
       <c r="G82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>701249326705417</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="13"/>
+        <v>452418920455107</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="10"/>
         <v>5.4346822819669776E+16</v>
       </c>
-      <c r="H82">
-        <f t="shared" si="9"/>
+      <c r="J82">
+        <f t="shared" si="11"/>
         <v>2173872912786790</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3820,23 +4474,31 @@
         <v>2.5271272611146445E+18</v>
       </c>
       <c r="E83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.6847515074097629E+17</v>
       </c>
       <c r="F83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1684751507409760</v>
       </c>
       <c r="G83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>1086936456393400</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="13"/>
+        <v>701249326705416</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="10"/>
         <v>8.4237575370488144E+16</v>
       </c>
-      <c r="H83">
-        <f t="shared" si="9"/>
+      <c r="J83">
+        <f t="shared" si="11"/>
         <v>3369503014819530</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3849,23 +4511,31 @@
         <v>3.9170472547276989E+18</v>
       </c>
       <c r="E84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.6113648364851325E+17</v>
       </c>
       <c r="F84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2611364836485130</v>
       </c>
       <c r="G84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
+        <v>1684751507409760</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="13"/>
+        <v>1086936456393400</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="10"/>
         <v>1.3056824182425662E+17</v>
       </c>
-      <c r="H84">
-        <f t="shared" si="9"/>
+      <c r="J84">
+        <f t="shared" si="11"/>
         <v>5222729672970270</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3878,23 +4548,31 @@
         <v>6.0714232448279337E+18</v>
       </c>
       <c r="E85">
-        <f t="shared" ref="E85:E102" si="10" xml:space="preserve"> base_damage * hits_1_round_behind ^ A84</f>
+        <f t="shared" ref="E85:E102" si="14" xml:space="preserve"> base_damage * hits_1_round_behind ^ A84</f>
         <v>4.0476154965519558E+17</v>
       </c>
       <c r="F85">
-        <f t="shared" ref="F85:F102" si="11">ROUNDUP(B85/base_damage, 0)</f>
+        <f t="shared" ref="F85:F102" si="15">ROUNDUP(B85/base_damage, 0)</f>
         <v>4047615496551960</v>
       </c>
       <c r="G85">
-        <f t="shared" ref="G85:G102" si="12">E85/2</f>
+        <f t="shared" si="12"/>
+        <v>2611364836485130</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="13"/>
+        <v>1684751507409760</v>
+      </c>
+      <c r="I85">
+        <f t="shared" ref="I85:I102" si="16">E85/2</f>
         <v>2.0238077482759779E+17</v>
       </c>
-      <c r="H85">
-        <f t="shared" ref="H85:H102" si="13">ROUNDUP(B85/explosion_shot_base, 0)</f>
+      <c r="J85">
+        <f t="shared" ref="J85:J102" si="17">ROUNDUP(B85/explosion_shot_base, 0)</f>
         <v>8095230993103910</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3907,23 +4585,31 @@
         <v>9.4107060294832968E+18</v>
       </c>
       <c r="E86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6.2738040196555315E+17</v>
       </c>
       <c r="F86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6273804019655530</v>
       </c>
       <c r="G86">
         <f t="shared" si="12"/>
-        <v>3.1369020098277658E+17</v>
+        <v>4047615496551960</v>
       </c>
       <c r="H86">
         <f t="shared" si="13"/>
+        <v>2611364836485130</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="16"/>
+        <v>3.1369020098277658E+17</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="17"/>
         <v>1.25476080393111E+16</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3936,23 +4622,31 @@
         <v>1.4586594345699115E+19</v>
       </c>
       <c r="E87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9.7243962304660762E+17</v>
       </c>
       <c r="F87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>9724396230466080</v>
       </c>
       <c r="G87">
         <f t="shared" si="12"/>
-        <v>4.8621981152330381E+17</v>
+        <v>6273804019655530</v>
       </c>
       <c r="H87">
         <f t="shared" si="13"/>
+        <v>4047615496551960</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="16"/>
+        <v>4.8621981152330381E+17</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="17"/>
         <v>1.94487924609322E+16</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3965,23 +4659,31 @@
         <v>2.2609221235833627E+19</v>
       </c>
       <c r="E88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.5072814157222418E+18</v>
       </c>
       <c r="F88">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.50728141572224E+16</v>
       </c>
       <c r="G88">
         <f t="shared" si="12"/>
-        <v>7.536407078611209E+17</v>
+        <v>9724396230466080</v>
       </c>
       <c r="H88">
         <f t="shared" si="13"/>
+        <v>6273804019655530</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="16"/>
+        <v>7.536407078611209E+17</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="17"/>
         <v>3.01456283144448E+16</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3994,23 +4696,31 @@
         <v>3.5044292915542127E+19</v>
       </c>
       <c r="E89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.3362861943694751E+18</v>
       </c>
       <c r="F89">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2.33628619436948E+16</v>
       </c>
       <c r="G89">
         <f t="shared" si="12"/>
-        <v>1.1681430971847375E+18</v>
+        <v>1.50728141572224E+16</v>
       </c>
       <c r="H89">
         <f t="shared" si="13"/>
+        <v>9724396230466080</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="16"/>
+        <v>1.1681430971847375E+18</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="17"/>
         <v>4.6725723887389504E+16</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4023,23 +4733,31 @@
         <v>5.4318654019090301E+19</v>
       </c>
       <c r="E90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3.6212436012726866E+18</v>
       </c>
       <c r="F90">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.6212436012726896E+16</v>
       </c>
       <c r="G90">
         <f t="shared" si="12"/>
-        <v>1.8106218006363433E+18</v>
+        <v>2.33628619436948E+16</v>
       </c>
       <c r="H90">
         <f t="shared" si="13"/>
+        <v>1.50728141572224E+16</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="16"/>
+        <v>1.8106218006363433E+18</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="17"/>
         <v>7.2424872025453696E+16</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4052,23 +4770,31 @@
         <v>8.4193913729589969E+19</v>
       </c>
       <c r="E91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>5.6129275819726643E+18</v>
       </c>
       <c r="F91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.61292758197266E+16</v>
       </c>
       <c r="G91">
         <f t="shared" si="12"/>
-        <v>2.8064637909863322E+18</v>
+        <v>3.6212436012726896E+16</v>
       </c>
       <c r="H91">
         <f t="shared" si="13"/>
+        <v>2.33628619436947E+16</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="16"/>
+        <v>2.8064637909863322E+18</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="17"/>
         <v>1.1225855163945299E+17</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4081,23 +4807,31 @@
         <v>1.3050056628086448E+20</v>
       </c>
       <c r="E92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8.7000377520576317E+18</v>
       </c>
       <c r="F92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>8.7000377520576304E+16</v>
       </c>
       <c r="G92">
         <f t="shared" si="12"/>
-        <v>4.3500188760288159E+18</v>
+        <v>5.6129275819726704E+16</v>
       </c>
       <c r="H92">
         <f t="shared" si="13"/>
+        <v>3.6212436012726896E+16</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="16"/>
+        <v>4.3500188760288159E+18</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="17"/>
         <v>1.7400075504115299E+17</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4110,23 +4844,31 @@
         <v>2.0227587773533992E+20</v>
       </c>
       <c r="E93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.3485058515689329E+19</v>
       </c>
       <c r="F93">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.3485058515689299E+17</v>
       </c>
       <c r="G93">
-        <f t="shared" si="12"/>
-        <v>6.7425292578446643E+18</v>
+        <f>ROUNDUP(B93/$E$4, 0)</f>
+        <v>8.7000377520576304E+16</v>
       </c>
       <c r="H93">
         <f t="shared" si="13"/>
+        <v>5.61292758197266E+16</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="16"/>
+        <v>6.7425292578446643E+18</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="17"/>
         <v>2.6970117031378701E+17</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4139,23 +4881,31 @@
         <v>3.1352761048977683E+20</v>
       </c>
       <c r="E94">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.0901840699318456E+19</v>
       </c>
       <c r="F94">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2.0901840699318499E+17</v>
       </c>
       <c r="G94">
-        <f t="shared" si="12"/>
-        <v>1.0450920349659228E+19</v>
+        <f t="shared" ref="G94:G102" si="18">ROUNDUP(B94/$E$4, 0)</f>
+        <v>1.3485058515689299E+17</v>
       </c>
       <c r="H94">
         <f t="shared" si="13"/>
+        <v>8.7000377520576304E+16</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="16"/>
+        <v>1.0450920349659228E+19</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="17"/>
         <v>4.1803681398636902E+17</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4168,23 +4918,31 @@
         <v>4.8596779625915423E+20</v>
       </c>
       <c r="E95">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3.2397853083943617E+19</v>
       </c>
       <c r="F95">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.2397853083943603E+17</v>
       </c>
       <c r="G95">
-        <f t="shared" si="12"/>
-        <v>1.6198926541971808E+19</v>
+        <f t="shared" si="18"/>
+        <v>2.0901840699318499E+17</v>
       </c>
       <c r="H95">
         <f t="shared" si="13"/>
+        <v>1.3485058515689299E+17</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="16"/>
+        <v>1.6198926541971808E+19</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="17"/>
         <v>6.4795706167887206E+17</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4197,23 +4955,31 @@
         <v>7.5325008420168912E+20</v>
       </c>
       <c r="E96">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>5.0216672280112611E+19</v>
       </c>
       <c r="F96">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>5.0216672280112602E+17</v>
       </c>
       <c r="G96">
-        <f t="shared" si="12"/>
-        <v>2.5108336140056306E+19</v>
+        <f t="shared" si="18"/>
+        <v>3.2397853083943603E+17</v>
       </c>
       <c r="H96">
         <f t="shared" si="13"/>
+        <v>2.0901840699318499E+17</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="16"/>
+        <v>2.5108336140056306E+19</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="17"/>
         <v>1.00433344560225E+18</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4226,23 +4992,31 @@
         <v>1.1675376305126184E+21</v>
       </c>
       <c r="E97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7.7835842034174558E+19</v>
       </c>
       <c r="F97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>7.7835842034174605E+17</v>
       </c>
       <c r="G97">
-        <f t="shared" si="12"/>
-        <v>3.8917921017087279E+19</v>
+        <f t="shared" si="18"/>
+        <v>5.0216672280112602E+17</v>
       </c>
       <c r="H97">
         <f t="shared" si="13"/>
+        <v>3.2397853083943603E+17</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="16"/>
+        <v>3.8917921017087279E+19</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="17"/>
         <v>1.55671684068349E+18</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4255,23 +5029,31 @@
         <v>1.8096833272945587E+21</v>
       </c>
       <c r="E98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.2064555515297058E+20</v>
       </c>
       <c r="F98">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.2064555515297101E+18</v>
       </c>
       <c r="G98">
-        <f t="shared" si="12"/>
-        <v>6.032277757648529E+19</v>
+        <f t="shared" si="18"/>
+        <v>7.7835842034174605E+17</v>
       </c>
       <c r="H98">
         <f t="shared" si="13"/>
+        <v>5.0216672280112602E+17</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="16"/>
+        <v>6.032277757648529E+19</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="17"/>
         <v>2.4129111030594099E+18</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4284,23 +5066,31 @@
         <v>2.8050091573065658E+21</v>
       </c>
       <c r="E99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.8700061048710437E+20</v>
       </c>
       <c r="F99">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1.87000610487104E+18</v>
       </c>
       <c r="G99">
-        <f t="shared" si="12"/>
-        <v>9.3500305243552186E+19</v>
+        <f t="shared" si="18"/>
+        <v>1.2064555515297101E+18</v>
       </c>
       <c r="H99">
         <f t="shared" si="13"/>
+        <v>7.7835842034174605E+17</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="16"/>
+        <v>9.3500305243552186E+19</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="17"/>
         <v>3.7400122097420902E+18</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4313,23 +5103,31 @@
         <v>4.3477641938251767E+21</v>
       </c>
       <c r="E100">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.8985094625501177E+20</v>
       </c>
       <c r="F100">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2.8985094625501199E+18</v>
       </c>
       <c r="G100">
-        <f t="shared" si="12"/>
-        <v>1.4492547312750589E+20</v>
+        <f t="shared" si="18"/>
+        <v>1.87000610487104E+18</v>
       </c>
       <c r="H100">
         <f t="shared" si="13"/>
+        <v>1.2064555515297101E+18</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="16"/>
+        <v>1.4492547312750589E+20</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="17"/>
         <v>5.7970189251002399E+18</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4342,23 +5140,31 @@
         <v>6.7390345004290251E+21</v>
       </c>
       <c r="E101">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>4.4926896669526832E+20</v>
       </c>
       <c r="F101">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>4.4926896669526799E+18</v>
       </c>
       <c r="G101">
-        <f t="shared" si="12"/>
-        <v>2.2463448334763416E+20</v>
+        <f t="shared" si="18"/>
+        <v>2.8985094625501199E+18</v>
       </c>
       <c r="H101">
         <f t="shared" si="13"/>
+        <v>1.87000610487104E+18</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="16"/>
+        <v>2.2463448334763416E+20</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="17"/>
         <v>8.9853793339053701E+18</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4371,19 +5177,27 @@
         <v>1.0445503475664988E+22</v>
       </c>
       <c r="E102">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6.9636689837766594E+20</v>
       </c>
       <c r="F102">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>6.9636689837766605E+18</v>
       </c>
       <c r="G102">
-        <f t="shared" si="12"/>
-        <v>3.4818344918883297E+20</v>
+        <f t="shared" si="18"/>
+        <v>4.4926896669526799E+18</v>
       </c>
       <c r="H102">
         <f t="shared" si="13"/>
+        <v>2.8985094625501199E+18</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="16"/>
+        <v>3.4818344918883297E+20</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="17"/>
         <v>1.39273379675533E+19</v>
       </c>
     </row>
@@ -4406,7 +5220,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5201,12 +6015,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5227,7 +6041,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5575,12 +6389,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5601,16 +6415,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5627,7 +6441,7 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -5635,7 +6449,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2">
         <f>D2</f>
@@ -5644,7 +6458,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -5652,7 +6466,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <f>A2</f>
@@ -5661,19 +6475,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6">
         <f>MAX(((H4-H2)+1 )*H3* H5, 1)</f>
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -5681,7 +6495,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9">
         <f xml:space="preserve"> H8 /H6</f>

</xml_diff>